<commit_message>
Included party data into the metrics and included leaders into the optimisation model
</commit_message>
<xml_diff>
--- a/AinBOptimisationdataModel_LF.xlsx
+++ b/AinBOptimisationdataModel_LF.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14280"/>
+    <workbookView xWindow="720" yWindow="720" windowWidth="22680" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Optimisation Model" sheetId="1" r:id="rId1"/>
-    <sheet name="To do" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Optimisation Model'!$N$2:$P$61</definedName>
@@ -79,13 +78,16 @@
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Optimisation Model'!$Z$14</definedName>
     <definedName name="solver_lhs60" localSheetId="0" hidden="1">'Optimisation Model'!$Z$68</definedName>
     <definedName name="solver_lhs61" localSheetId="0" hidden="1">'Optimisation Model'!$Z$69</definedName>
-    <definedName name="solver_lhs62" localSheetId="0" hidden="1">'Optimisation Model'!$Z$70</definedName>
-    <definedName name="solver_lhs63" localSheetId="0" hidden="1">'Optimisation Model'!$Z$71</definedName>
-    <definedName name="solver_lhs64" localSheetId="0" hidden="1">'Optimisation Model'!$Z$72</definedName>
-    <definedName name="solver_lhs65" localSheetId="0" hidden="1">'Optimisation Model'!$Z$73</definedName>
-    <definedName name="solver_lhs66" localSheetId="0" hidden="1">'Optimisation Model'!$Z$74</definedName>
-    <definedName name="solver_lhs67" localSheetId="0" hidden="1">'Optimisation Model'!$Z$75</definedName>
+    <definedName name="solver_lhs62" localSheetId="0" hidden="1">'Optimisation Model'!$Z$7</definedName>
+    <definedName name="solver_lhs63" localSheetId="0" hidden="1">'Optimisation Model'!$Z$70</definedName>
+    <definedName name="solver_lhs64" localSheetId="0" hidden="1">'Optimisation Model'!$Z$71</definedName>
+    <definedName name="solver_lhs65" localSheetId="0" hidden="1">'Optimisation Model'!$Z$72</definedName>
+    <definedName name="solver_lhs66" localSheetId="0" hidden="1">'Optimisation Model'!$Z$73</definedName>
+    <definedName name="solver_lhs67" localSheetId="0" hidden="1">'Optimisation Model'!$Z$74</definedName>
+    <definedName name="solver_lhs68" localSheetId="0" hidden="1">'Optimisation Model'!$Z$75</definedName>
+    <definedName name="solver_lhs69" localSheetId="0" hidden="1">'Optimisation Model'!$Z$8</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Optimisation Model'!$Z$15</definedName>
+    <definedName name="solver_lhs70" localSheetId="0" hidden="1">'Optimisation Model'!$Z$9</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Optimisation Model'!$Z$16</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Optimisation Model'!$Z$17</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
@@ -95,8 +97,8 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">67</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">'Optimisation Model'!$Z$4</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">70</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Optimisation Model'!$Z$3</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">5</definedName>
@@ -157,13 +159,16 @@
     <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel60" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel61" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel62" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel62" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel63" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel64" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel65" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel66" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel67" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel68" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel69" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel70" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">binary</definedName>
@@ -224,13 +229,16 @@
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Optimisation Model'!$AA$14</definedName>
     <definedName name="solver_rhs60" localSheetId="0" hidden="1">'Optimisation Model'!$AA$68</definedName>
     <definedName name="solver_rhs61" localSheetId="0" hidden="1">'Optimisation Model'!$AA$69</definedName>
-    <definedName name="solver_rhs62" localSheetId="0" hidden="1">'Optimisation Model'!$AA$70</definedName>
-    <definedName name="solver_rhs63" localSheetId="0" hidden="1">'Optimisation Model'!$AA$71</definedName>
-    <definedName name="solver_rhs64" localSheetId="0" hidden="1">'Optimisation Model'!$AA$72</definedName>
-    <definedName name="solver_rhs65" localSheetId="0" hidden="1">'Optimisation Model'!$AA$73</definedName>
-    <definedName name="solver_rhs66" localSheetId="0" hidden="1">'Optimisation Model'!$AA$74</definedName>
-    <definedName name="solver_rhs67" localSheetId="0" hidden="1">'Optimisation Model'!$AA$75</definedName>
+    <definedName name="solver_rhs62" localSheetId="0" hidden="1">'Optimisation Model'!$AA$7</definedName>
+    <definedName name="solver_rhs63" localSheetId="0" hidden="1">'Optimisation Model'!$AA$70</definedName>
+    <definedName name="solver_rhs64" localSheetId="0" hidden="1">'Optimisation Model'!$AA$71</definedName>
+    <definedName name="solver_rhs65" localSheetId="0" hidden="1">'Optimisation Model'!$AA$72</definedName>
+    <definedName name="solver_rhs66" localSheetId="0" hidden="1">'Optimisation Model'!$AA$73</definedName>
+    <definedName name="solver_rhs67" localSheetId="0" hidden="1">'Optimisation Model'!$AA$74</definedName>
+    <definedName name="solver_rhs68" localSheetId="0" hidden="1">'Optimisation Model'!$AA$75</definedName>
+    <definedName name="solver_rhs69" localSheetId="0" hidden="1">'Optimisation Model'!$AA$8</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Optimisation Model'!$AA$15</definedName>
+    <definedName name="solver_rhs70" localSheetId="0" hidden="1">'Optimisation Model'!$AA$9</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Optimisation Model'!$AA$16</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">'Optimisation Model'!$AA$17</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -257,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="157">
   <si>
     <t>node</t>
   </si>
@@ -721,17 +729,20 @@
     <t>One team - 60</t>
   </si>
   <si>
-    <t>Include Party Data</t>
-  </si>
-  <si>
-    <t>Include clique/clusters</t>
+    <t>Leader Design</t>
+  </si>
+  <si>
+    <t>Leader Lobby</t>
+  </si>
+  <si>
+    <t>Leader Infl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -789,6 +800,22 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -840,8 +867,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -860,7 +891,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1142,7 +1177,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P34" sqref="P34"/>
+      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1161,6 +1196,9 @@
     <col min="20" max="20" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.83203125" customWidth="1"/>
+    <col min="26" max="26" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
@@ -1251,28 +1289,28 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <v>0.14274341870493279</v>
+        <v>0.2847986837409866</v>
       </c>
       <c r="I2">
-        <v>0.82791182848861011</v>
+        <v>1.6518323656977223</v>
       </c>
       <c r="J2">
-        <v>0.46579604739312669</v>
+        <v>0.44086387350270534</v>
       </c>
       <c r="K2">
-        <v>2.7016170748801347</v>
+        <v>2.557010466315691</v>
       </c>
       <c r="L2">
-        <v>0.81287301913974075</v>
+        <v>0.39257460382794812</v>
       </c>
       <c r="M2">
-        <v>4.714663511010496</v>
+        <v>2.2769327022020991</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -1283,7 +1321,7 @@
       </c>
       <c r="R2">
         <f>O2*J2</f>
-        <v>0</v>
+        <v>0.44086387350270534</v>
       </c>
       <c r="S2">
         <f>L2*P2</f>
@@ -1295,7 +1333,7 @@
       </c>
       <c r="U2">
         <f>O2*C2</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="V2">
         <f>P2*C2</f>
@@ -1325,22 +1363,22 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>0.62442820621891537</v>
+        <v>0.2811356412437831</v>
       </c>
       <c r="I3">
-        <v>1.3929552292575804</v>
+        <v>0.62714873815920846</v>
       </c>
       <c r="J3">
-        <v>0.4709516619834217</v>
+        <v>0.39444127085397485</v>
       </c>
       <c r="K3">
-        <v>1.0505844767322483</v>
+        <v>0.87990745036655926</v>
       </c>
       <c r="L3">
-        <v>1.1112734457616742</v>
+        <v>0.59225468915233481</v>
       </c>
       <c r="M3">
-        <v>2.4789946097760422</v>
+        <v>1.3211835373398237</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1374,6 +1412,13 @@
       <c r="V3">
         <f t="shared" ref="V3:V61" si="5">P3*C3</f>
         <v>0</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z3">
+        <f>SUM('Optimisation Model'!Q2:Q61)+SUM('Optimisation Model'!R2:R61)+SUM('Optimisation Model'!S2:S61)</f>
+        <v>9.1738012645278388</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -1399,22 +1444,22 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>0.41387071083721366</v>
+        <v>0.31089914216744274</v>
       </c>
       <c r="I4">
-        <v>2.400450122855839</v>
+        <v>1.8032150245711678</v>
       </c>
       <c r="J4">
-        <v>0.37464267019177389</v>
+        <v>0.3498570680767098</v>
       </c>
       <c r="K4">
-        <v>2.1729274871122883</v>
+        <v>2.0291709948449168</v>
       </c>
       <c r="L4">
-        <v>0.6842971804898127</v>
+        <v>0.21685943609796257</v>
       </c>
       <c r="M4">
-        <v>3.9689236468409135</v>
+        <v>1.2577847293681828</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1449,15 +1494,8 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z4">
-        <f>SUM('Optimisation Model'!Q2:Q61)+SUM('Optimisation Model'!R2:R61)+SUM('Optimisation Model'!S2:S61)</f>
-        <v>15.101441333689664</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:28" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1480,22 +1518,22 @@
         <v>4</v>
       </c>
       <c r="H5">
-        <v>0.15924828044222089</v>
+        <v>3.184965608844418E-2</v>
       </c>
       <c r="I5">
-        <v>1.5394000442748019</v>
+        <v>0.30788000885496042</v>
       </c>
       <c r="J5">
-        <v>0.29581393141579115</v>
+        <v>0.12741648165722569</v>
       </c>
       <c r="K5">
-        <v>2.8595346703526481</v>
+        <v>1.2316926560198482</v>
       </c>
       <c r="L5">
-        <v>0.75779348168513894</v>
+        <v>0.37655869633702777</v>
       </c>
       <c r="M5">
-        <v>7.3253369896230094</v>
+        <v>3.6400673979246019</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1530,6 +1568,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
+      <c r="Z5" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1554,22 +1597,22 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>0.32355835350033152</v>
+        <v>9.2836670700066307E-2</v>
       </c>
       <c r="I6">
-        <v>1.0425769168344015</v>
+        <v>0.29914038336688031</v>
       </c>
       <c r="J6">
-        <v>0.28826597409545551</v>
+        <v>0.15167002600181859</v>
       </c>
       <c r="K6">
-        <v>0.92885702764091216</v>
+        <v>0.48871452822808209</v>
       </c>
       <c r="L6">
-        <v>0.75591241989624658</v>
+        <v>0.42618248397924935</v>
       </c>
       <c r="M6">
-        <v>2.435717797443461</v>
+        <v>1.3732546705998034</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1603,6 +1646,15 @@
       <c r="V6">
         <f t="shared" si="5"/>
         <v>0</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA6" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB6" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -1628,22 +1680,22 @@
         <v>2</v>
       </c>
       <c r="H7">
-        <v>0.69186645377901723</v>
+        <v>0.30712329075580341</v>
       </c>
       <c r="I7">
-        <v>1.8240115599628637</v>
+        <v>0.80968867562893632</v>
       </c>
       <c r="J7">
-        <v>0.61637421448082108</v>
+        <v>0.30109514033778301</v>
       </c>
       <c r="K7">
-        <v>1.6249865654494375</v>
+        <v>0.79379627907233707</v>
       </c>
       <c r="L7">
-        <v>1.0059124198962466</v>
+        <v>0.62618248397924936</v>
       </c>
       <c r="M7">
-        <v>2.6519509251810138</v>
+        <v>1.6508447304907483</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1652,7 +1704,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
@@ -1664,7 +1716,7 @@
       </c>
       <c r="S7">
         <f t="shared" si="2"/>
-        <v>1.0059124198962466</v>
+        <v>0</v>
       </c>
       <c r="T7">
         <f t="shared" si="3"/>
@@ -1676,10 +1728,23 @@
       </c>
       <c r="V7">
         <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" ht="16" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z7" s="7">
+        <f>N31</f>
+        <v>1</v>
+      </c>
+      <c r="AA7" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB7" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -1702,39 +1767,39 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>0.99267781004965383</v>
+        <v>0.69853556200993083</v>
       </c>
       <c r="I8">
-        <v>1.9191770994293307</v>
+        <v>1.3505020865525328</v>
       </c>
       <c r="J8">
-        <v>1.0063229666884297</v>
+        <v>0.62374130788749327</v>
       </c>
       <c r="K8">
-        <v>1.9455577355976306</v>
+        <v>1.2058998619158203</v>
       </c>
       <c r="L8">
-        <v>1.166808486498752</v>
+        <v>0.55836169729975038</v>
       </c>
       <c r="M8">
-        <v>2.2558297405642538</v>
+        <v>1.0794992814461839</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.69853556200993083</v>
       </c>
       <c r="R8">
         <f t="shared" si="1"/>
-        <v>1.0063229666884297</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <f t="shared" si="2"/>
@@ -1742,21 +1807,29 @@
       </c>
       <c r="T8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="U8">
         <f t="shared" si="4"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="V8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Z8" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="AA8" s="10"/>
-      <c r="AB8" s="10"/>
+      <c r="Y8" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z8" s="7">
+        <f>O34</f>
+        <v>1</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -1781,22 +1854,22 @@
         <v>2</v>
       </c>
       <c r="H9">
-        <v>0.41521941679637253</v>
+        <v>0.13929388335927451</v>
       </c>
       <c r="I9">
-        <v>12.041363087094803</v>
+        <v>4.0395226174189611</v>
       </c>
       <c r="J9">
-        <v>0.29174054284018647</v>
+        <v>0.15305985349971105</v>
       </c>
       <c r="K9">
-        <v>8.4604757423654071</v>
+        <v>4.4387357514916204</v>
       </c>
       <c r="L9">
-        <v>0.84424914698965514</v>
+        <v>0.46884982939793102</v>
       </c>
       <c r="M9">
-        <v>24.4832252627</v>
+        <v>13.59664505254</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1805,7 +1878,7 @@
         <v>0</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
@@ -1817,7 +1890,7 @@
       </c>
       <c r="S9">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.46884982939793102</v>
       </c>
       <c r="T9">
         <f t="shared" si="3"/>
@@ -1829,16 +1902,20 @@
       </c>
       <c r="V9">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="Z9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="AB9" s="5" t="s">
-        <v>82</v>
+        <v>1</v>
+      </c>
+      <c r="Y9" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z9" s="7">
+        <f>P20</f>
+        <v>1</v>
+      </c>
+      <c r="AA9" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB9" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
@@ -1864,22 +1941,22 @@
         <v>4</v>
       </c>
       <c r="H10">
-        <v>0.7487554253388925</v>
+        <v>0.20600108506777848</v>
       </c>
       <c r="I10">
-        <v>2.4126563705364314</v>
+        <v>0.66378127410728616</v>
       </c>
       <c r="J10">
-        <v>0.29232707359008853</v>
+        <v>0.16238537489058091</v>
       </c>
       <c r="K10">
-        <v>0.94194279267917413</v>
+        <v>0.52324176353631624</v>
       </c>
       <c r="L10">
-        <v>0.81245045677231564</v>
+        <v>0.46249009135446312</v>
       </c>
       <c r="M10">
-        <v>2.6178959162663502</v>
+        <v>1.4902458499199367</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1951,22 +2028,22 @@
         <v>2</v>
       </c>
       <c r="H11">
-        <v>0.29353668076128825</v>
+        <v>0.11495733615225766</v>
       </c>
       <c r="I11">
-        <v>1.2160805345824799</v>
+        <v>0.47625182120221027</v>
       </c>
       <c r="J11">
-        <v>0.42968819588101648</v>
+        <v>0.20823891471604311</v>
       </c>
       <c r="K11">
-        <v>1.7801368115070682</v>
+        <v>0.86270407525217851</v>
       </c>
       <c r="L11">
-        <v>0.73889157432884656</v>
+        <v>0.42277831486576933</v>
       </c>
       <c r="M11">
-        <v>3.0611222365052213</v>
+        <v>1.7515101615867585</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2038,22 +2115,22 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <v>0.23727835325469404</v>
+        <v>0.27558067065093883</v>
       </c>
       <c r="I12">
-        <v>0.98301032062658955</v>
+        <v>1.1416913498396037</v>
       </c>
       <c r="J12">
-        <v>0.26209453779049663</v>
+        <v>0.34120145147983494</v>
       </c>
       <c r="K12">
-        <v>1.0858202279892002</v>
+        <v>1.4135488704164589</v>
       </c>
       <c r="L12">
-        <v>0.85411712343898238</v>
+        <v>0.37582342468779645</v>
       </c>
       <c r="M12">
-        <v>3.5384852256757839</v>
+        <v>1.5569827594208709</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2125,22 +2202,22 @@
         <v>3</v>
       </c>
       <c r="H13">
-        <v>0.20264815478232964</v>
+        <v>0.26865463095646591</v>
       </c>
       <c r="I13">
-        <v>0.45206126836058153</v>
+        <v>0.59930648444134704</v>
       </c>
       <c r="J13">
-        <v>0.39033212628319902</v>
+        <v>0.374314668695098</v>
       </c>
       <c r="K13">
-        <v>0.87074089709329006</v>
+        <v>0.8350096455506032</v>
       </c>
       <c r="L13">
-        <v>0.66961374675627117</v>
+        <v>0.28892274935125423</v>
       </c>
       <c r="M13">
-        <v>1.4937537427639895</v>
+        <v>0.64451997932202865</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2212,22 +2289,22 @@
         <v>5</v>
       </c>
       <c r="H14">
-        <v>0.75007604063175348</v>
+        <v>0.41251520812635073</v>
       </c>
       <c r="I14">
-        <v>1.9774731980291684</v>
+        <v>1.0875400941512883</v>
       </c>
       <c r="J14">
-        <v>0.3219038536211366</v>
+        <v>0.35603426872118205</v>
       </c>
       <c r="K14">
-        <v>0.84865561409208745</v>
+        <v>0.93863579935584363</v>
       </c>
       <c r="L14">
-        <v>0.86127344576167419</v>
+        <v>0.39225468915233486</v>
       </c>
       <c r="M14">
-        <v>2.2706299933716867</v>
+        <v>1.0341259986743374</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2299,22 +2376,22 @@
         <v>3</v>
       </c>
       <c r="H15">
-        <v>0.28125</v>
+        <v>0.32499999999999996</v>
       </c>
       <c r="I15">
-        <v>0.42927631578947367</v>
+        <v>0.4960526315789473</v>
       </c>
       <c r="J15">
-        <v>0.48476902220148299</v>
+        <v>0.33330154827453273</v>
       </c>
       <c r="K15">
-        <v>0.73991061283384252</v>
+        <v>0.50872341578744473</v>
       </c>
       <c r="L15">
-        <v>0.41666666666666669</v>
+        <v>0.4933333333333334</v>
       </c>
       <c r="M15">
-        <v>0.63596491228070184</v>
+        <v>0.75298245614035098</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2354,7 +2431,7 @@
       </c>
       <c r="Z15" s="7">
         <f>SUM('Optimisation Model'!V2:V61)</f>
-        <v>29.5</v>
+        <v>30</v>
       </c>
       <c r="AA15" s="7">
         <v>30</v>
@@ -2386,22 +2463,22 @@
         <v>2</v>
       </c>
       <c r="H16">
-        <v>0.1875</v>
+        <v>0.2</v>
       </c>
       <c r="I16">
-        <v>1.8125</v>
+        <v>1.9333333333333336</v>
       </c>
       <c r="J16">
-        <v>0.13685603828609472</v>
+        <v>0.15777271834474105</v>
       </c>
       <c r="K16">
-        <v>1.322941703432249</v>
+        <v>1.5251362773324968</v>
       </c>
       <c r="L16">
-        <v>0.75516919908721547</v>
+        <v>0.27603383981744312</v>
       </c>
       <c r="M16">
-        <v>7.2999689245097494</v>
+        <v>2.6683271182352835</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2441,7 +2518,7 @@
       </c>
       <c r="Z16" s="7">
         <f>'Optimisation Model'!N2+'Optimisation Model'!O2+'Optimisation Model'!P2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA16" s="7">
         <v>1</v>
@@ -2473,22 +2550,22 @@
         <v>5</v>
       </c>
       <c r="H17">
-        <v>0.41613244335648786</v>
+        <v>0.26760148867129757</v>
       </c>
       <c r="I17">
-        <v>1.3408712063709052</v>
+        <v>0.86227146349640327</v>
       </c>
       <c r="J17">
-        <v>0.31725948204617416</v>
+        <v>0.2966007625154396</v>
       </c>
       <c r="K17">
-        <v>1.0222805532598944</v>
+        <v>0.95571356810530539</v>
       </c>
       <c r="L17">
-        <v>0.8760726736390454</v>
+        <v>0.42021453472780906</v>
       </c>
       <c r="M17">
-        <v>2.8229008372813684</v>
+        <v>1.354024611900718</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -2560,22 +2637,22 @@
         <v>2</v>
       </c>
       <c r="H18">
-        <v>0.45537927266474282</v>
+        <v>0.34732585453294856</v>
       </c>
       <c r="I18">
-        <v>0.57417386553380612</v>
+        <v>0.43793259919371774</v>
       </c>
       <c r="J18">
-        <v>0.94890679620103502</v>
+        <v>0.63410817302586864</v>
       </c>
       <c r="K18">
-        <v>1.1964476995578268</v>
+        <v>0.7995276964239213</v>
       </c>
       <c r="L18">
-        <v>0.8920162788156889</v>
+        <v>0.43340325576313776</v>
       </c>
       <c r="M18">
-        <v>1.124716177637173</v>
+        <v>0.54646497465786936</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2647,22 +2724,22 @@
         <v>5</v>
       </c>
       <c r="H19">
-        <v>0.63400192764169949</v>
+        <v>0.21117538552833989</v>
       </c>
       <c r="I19">
-        <v>1.6714596274190261</v>
+        <v>0.55673510730198705</v>
       </c>
       <c r="J19">
-        <v>0.36717937088417058</v>
+        <v>0.19232629380821376</v>
       </c>
       <c r="K19">
-        <v>0.96801834142190424</v>
+        <v>0.50704204731256353</v>
       </c>
       <c r="L19">
-        <v>1.0041201744260613</v>
+        <v>0.57582403488521228</v>
       </c>
       <c r="M19">
-        <v>2.64722591439598</v>
+        <v>1.5180815465155597</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2734,22 +2811,22 @@
         <v>2</v>
       </c>
       <c r="H20">
-        <v>0.976819835877072</v>
+        <v>0.63286396717541438</v>
       </c>
       <c r="I20">
-        <v>1.4909355389702679</v>
+        <v>0.96595026568879039</v>
       </c>
       <c r="J20">
-        <v>0.94200266564282231</v>
+        <v>0.55255864201470462</v>
       </c>
       <c r="K20">
-        <v>1.4377935422969395</v>
+        <v>0.8433789799171808</v>
       </c>
       <c r="L20">
-        <v>1.1290203634979541</v>
+        <v>0.71080407269959078</v>
       </c>
       <c r="M20">
-        <v>1.7232416074442458</v>
+        <v>1.0849114793835859</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2758,7 +2835,7 @@
         <v>0</v>
       </c>
       <c r="P20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20">
         <f t="shared" si="0"/>
@@ -2770,7 +2847,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.71080407269959078</v>
       </c>
       <c r="T20">
         <f t="shared" si="3"/>
@@ -2782,7 +2859,7 @@
       </c>
       <c r="V20">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y20" s="6" t="s">
         <v>98</v>
@@ -2821,35 +2898,35 @@
         <v>2</v>
       </c>
       <c r="H21">
-        <v>1.0191102440155124</v>
+        <v>0.71319704880310253</v>
       </c>
       <c r="I21">
-        <v>2.2733997751115278</v>
+        <v>1.5909780319453826</v>
       </c>
       <c r="J21">
-        <v>0.74830934867178134</v>
+        <v>0.63568737583234891</v>
       </c>
       <c r="K21">
-        <v>1.6693054701139738</v>
+        <v>1.4180718383952398</v>
       </c>
       <c r="L21">
-        <v>1.1133586177833967</v>
+        <v>0.57767172355667928</v>
       </c>
       <c r="M21">
-        <v>2.4836461473629621</v>
+        <v>1.2886523063956692</v>
       </c>
       <c r="N21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21">
         <v>0</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.71319704880310253</v>
       </c>
       <c r="R21">
         <f t="shared" si="1"/>
@@ -2857,11 +2934,11 @@
       </c>
       <c r="S21">
         <f t="shared" si="2"/>
-        <v>1.1133586177833967</v>
+        <v>0</v>
       </c>
       <c r="T21">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U21">
         <f t="shared" si="4"/>
@@ -2869,14 +2946,14 @@
       </c>
       <c r="V21">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="Y21" s="6" t="s">
         <v>99</v>
       </c>
       <c r="Z21" s="7">
         <f>'Optimisation Model'!N7+'Optimisation Model'!O7+'Optimisation Model'!P7</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA21" s="7">
         <v>1</v>
@@ -2908,28 +2985,28 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>1.0877093945093697</v>
+        <v>0.66129187890187402</v>
       </c>
       <c r="I22">
-        <v>1.6601880231985116</v>
+        <v>1.0093402362186499</v>
       </c>
       <c r="J22">
-        <v>1.2745191290813436</v>
+        <v>0.77647431829920421</v>
       </c>
       <c r="K22">
-        <v>1.9453186707031034</v>
+        <v>1.1851450121408906</v>
       </c>
       <c r="L22">
-        <v>1.2388915743288464</v>
+        <v>0.62277831486576929</v>
       </c>
       <c r="M22">
-        <v>1.8909397713440288</v>
+        <v>0.95055637532143733</v>
       </c>
       <c r="N22">
         <v>0</v>
       </c>
       <c r="O22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P22">
         <v>0</v>
@@ -2940,7 +3017,7 @@
       </c>
       <c r="R22">
         <f t="shared" si="1"/>
-        <v>1.2745191290813436</v>
+        <v>0</v>
       </c>
       <c r="S22">
         <f t="shared" si="2"/>
@@ -2952,7 +3029,7 @@
       </c>
       <c r="U22">
         <f t="shared" si="4"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V22">
         <f t="shared" si="5"/>
@@ -2995,22 +3072,22 @@
         <v>2</v>
       </c>
       <c r="H23">
-        <v>0.79935413738212591</v>
+        <v>0.35049582747642516</v>
       </c>
       <c r="I23">
-        <v>1.5454179989387766</v>
+        <v>0.67762526645442189</v>
       </c>
       <c r="J23">
-        <v>0.87193112317562138</v>
+        <v>0.57301487351267288</v>
       </c>
       <c r="K23">
-        <v>1.6857335048062012</v>
+        <v>1.1078287554578341</v>
       </c>
       <c r="L23">
-        <v>1.069471186482517</v>
+        <v>0.64889423729650342</v>
       </c>
       <c r="M23">
-        <v>2.0676442938661994</v>
+        <v>1.2545288587732399</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3019,7 +3096,7 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -3031,7 +3108,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.64889423729650342</v>
       </c>
       <c r="T23">
         <f t="shared" si="3"/>
@@ -3043,14 +3120,14 @@
       </c>
       <c r="V23">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y23" s="6" t="s">
         <v>101</v>
       </c>
       <c r="Z23" s="7">
         <f>'Optimisation Model'!N9+'Optimisation Model'!O9+'Optimisation Model'!P9</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" s="7">
         <v>1</v>
@@ -3082,22 +3159,22 @@
         <v>4</v>
       </c>
       <c r="H24">
-        <v>0.15266321686203538</v>
+        <v>0.2586576433724071</v>
       </c>
       <c r="I24">
-        <v>0.88544665779980514</v>
+        <v>1.500214331559961</v>
       </c>
       <c r="J24">
-        <v>0.34106851525165061</v>
+        <v>0.39097286064611486</v>
       </c>
       <c r="K24">
-        <v>1.9781973884595734</v>
+        <v>2.2676425917474661</v>
       </c>
       <c r="L24">
-        <v>0.85717036050852335</v>
+        <v>0.37643407210170471</v>
       </c>
       <c r="M24">
-        <v>4.9715880909494352</v>
+        <v>2.183317618189887</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -3169,28 +3246,28 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <v>0.37097076545094926</v>
+        <v>0.31481915309018982</v>
       </c>
       <c r="I25">
-        <v>1.5368788854396469</v>
+        <v>1.3042507770879292</v>
       </c>
       <c r="J25">
-        <v>0.49372731115065732</v>
+        <v>0.37627880324814178</v>
       </c>
       <c r="K25">
-        <v>2.0454417176241515</v>
+        <v>1.5588693277423016</v>
       </c>
       <c r="L25">
-        <v>0.80604115286038991</v>
+        <v>0.406208230572078</v>
       </c>
       <c r="M25">
-        <v>3.3393133475644725</v>
+        <v>1.6828626695128945</v>
       </c>
       <c r="N25">
         <v>0</v>
       </c>
       <c r="O25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25">
         <v>0</v>
@@ -3201,7 +3278,7 @@
       </c>
       <c r="R25">
         <f t="shared" si="1"/>
-        <v>0.49372731115065732</v>
+        <v>0</v>
       </c>
       <c r="S25">
         <f t="shared" si="2"/>
@@ -3213,7 +3290,7 @@
       </c>
       <c r="U25">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V25">
         <f t="shared" si="5"/>
@@ -3256,22 +3333,22 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>0.59154934277207616</v>
+        <v>0.41518486855441528</v>
       </c>
       <c r="I26">
-        <v>1.1436620626926806</v>
+        <v>0.8026907458718695</v>
       </c>
       <c r="J26">
-        <v>0.87610261243022935</v>
+        <v>0.48074407527512208</v>
       </c>
       <c r="K26">
-        <v>1.6937983840317767</v>
+        <v>0.92943854553190264</v>
       </c>
       <c r="L26">
-        <v>1.0750018669952581</v>
+        <v>0.65000037339905159</v>
       </c>
       <c r="M26">
-        <v>2.0783369428574989</v>
+        <v>1.2566673885714996</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -3280,7 +3357,7 @@
         <v>0</v>
       </c>
       <c r="P26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26">
         <f t="shared" si="0"/>
@@ -3292,7 +3369,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.65000037339905159</v>
       </c>
       <c r="T26">
         <f t="shared" si="3"/>
@@ -3304,7 +3381,7 @@
       </c>
       <c r="V26">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y26" s="6" t="s">
         <v>104</v>
@@ -3343,22 +3420,22 @@
         <v>4</v>
       </c>
       <c r="H27">
-        <v>0.71160900282766615</v>
+        <v>0.42669680056553327</v>
       </c>
       <c r="I27">
-        <v>2.2929623424447021</v>
+        <v>1.3749119129333849</v>
       </c>
       <c r="J27">
-        <v>0.3715794861731907</v>
+        <v>0.38499543083291282</v>
       </c>
       <c r="K27">
-        <v>1.1973116776691699</v>
+        <v>1.2405408326838301</v>
       </c>
       <c r="L27">
-        <v>0.9552123470381505</v>
+        <v>0.42104246940763007</v>
       </c>
       <c r="M27">
-        <v>3.0779064515673737</v>
+        <v>1.3566924014245858</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -3415,7 +3492,7 @@
         <v>27</v>
       </c>
       <c r="C28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>1</v>
@@ -3429,20 +3506,20 @@
       <c r="G28">
         <v>4</v>
       </c>
-      <c r="H28">
-        <v>0</v>
+      <c r="H28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="I28" t="e">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J28" t="e">
         <v>#N/A</v>
-      </c>
-      <c r="J28">
-        <v>7.8196195752840147E-2</v>
       </c>
       <c r="K28" t="e">
         <v>#N/A</v>
       </c>
-      <c r="L28">
-        <v>1.0833333333333333</v>
+      <c r="L28" t="e">
+        <v>#N/A</v>
       </c>
       <c r="M28" t="e">
         <v>#N/A</v>
@@ -3454,19 +3531,16 @@
         <v>0</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R28">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="S28">
-        <f t="shared" si="2"/>
-        <v>1.0833333333333333</v>
+        <v>0</v>
       </c>
       <c r="T28">
         <f t="shared" si="3"/>
@@ -3478,7 +3552,7 @@
       </c>
       <c r="V28">
         <f t="shared" si="5"/>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Y28" s="6" t="s">
         <v>106</v>
@@ -3517,22 +3591,22 @@
         <v>3</v>
       </c>
       <c r="H29">
-        <v>0.67656668496513717</v>
+        <v>0.38218833699302746</v>
       </c>
       <c r="I29">
-        <v>1.5092641433837675</v>
+        <v>0.85257398252290739</v>
       </c>
       <c r="J29">
-        <v>0.50757964035571201</v>
+        <v>0.3151530682634972</v>
       </c>
       <c r="K29">
-        <v>1.1322930438704344</v>
+        <v>0.70303376766472447</v>
       </c>
       <c r="L29">
-        <v>0.62794708008960454</v>
+        <v>0.17558941601792089</v>
       </c>
       <c r="M29">
-        <v>1.4008050248152717</v>
+        <v>0.39169946650151583</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -3604,22 +3678,22 @@
         <v>2</v>
       </c>
       <c r="H30">
-        <v>0.79117810107436704</v>
+        <v>0.3207356202148734</v>
       </c>
       <c r="I30">
-        <v>1.3496567606562733</v>
+        <v>0.54713723448419582</v>
       </c>
       <c r="J30">
-        <v>0.68684730664653826</v>
+        <v>0.45352680144649449</v>
       </c>
       <c r="K30">
-        <v>1.1716806995735065</v>
+        <v>0.77366336717343187</v>
       </c>
       <c r="L30">
-        <v>0.96134806993555899</v>
+        <v>0.55226961398711183</v>
       </c>
       <c r="M30">
-        <v>1.6399467075371301</v>
+        <v>0.94210698856624964</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -3691,35 +3765,35 @@
         <v>2</v>
       </c>
       <c r="H31">
-        <v>0.50959682246862614</v>
+        <v>0.58316936449372525</v>
       </c>
       <c r="I31">
-        <v>14.778307851590158</v>
+        <v>16.911911570318033</v>
       </c>
       <c r="J31">
-        <v>0.58485877695958088</v>
+        <v>0.58848896532928707</v>
       </c>
       <c r="K31">
-        <v>16.960904531827847</v>
+        <v>17.066179994549326</v>
       </c>
       <c r="L31">
-        <v>1.2362734457616742</v>
+        <v>0.65225468915233487</v>
       </c>
       <c r="M31">
-        <v>35.851929927088555</v>
+        <v>18.915385985417711</v>
       </c>
       <c r="N31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31">
         <v>0</v>
       </c>
       <c r="P31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q31">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.58316936449372525</v>
       </c>
       <c r="R31">
         <f t="shared" si="1"/>
@@ -3727,11 +3801,11 @@
       </c>
       <c r="S31">
         <f t="shared" si="2"/>
-        <v>1.2362734457616742</v>
+        <v>0</v>
       </c>
       <c r="T31">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31">
         <f t="shared" si="4"/>
@@ -3739,7 +3813,7 @@
       </c>
       <c r="V31">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y31" s="6" t="s">
         <v>109</v>
@@ -3778,22 +3852,22 @@
         <v>2</v>
       </c>
       <c r="H32">
-        <v>0.35597528041512944</v>
+        <v>0.27119505608302591</v>
       </c>
       <c r="I32">
-        <v>2.0646566264077504</v>
+        <v>1.5729313252815502</v>
       </c>
       <c r="J32">
-        <v>0.22829692769409451</v>
+        <v>0.30040968016854697</v>
       </c>
       <c r="K32">
-        <v>1.3241221806257482</v>
+        <v>1.7423761449775723</v>
       </c>
       <c r="L32">
-        <v>0.88925762045231072</v>
+        <v>0.38285152409046214</v>
       </c>
       <c r="M32">
-        <v>5.1576941986234015</v>
+        <v>2.2205388397246804</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -3865,22 +3939,22 @@
         <v>5</v>
       </c>
       <c r="H33">
-        <v>0.22336404854413491</v>
+        <v>4.4672809708826984E-2</v>
       </c>
       <c r="I33">
-        <v>0.71972860086443469</v>
+        <v>0.14394572017288695</v>
       </c>
       <c r="J33">
-        <v>0.25410993211033261</v>
+        <v>0.11982579102595142</v>
       </c>
       <c r="K33">
-        <v>0.81879867013329399</v>
+        <v>0.38610532663917679</v>
       </c>
       <c r="L33">
-        <v>0.78632504185601537</v>
+        <v>0.43226500837120313</v>
       </c>
       <c r="M33">
-        <v>2.5337140237582716</v>
+        <v>1.3928539158627655</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -3952,31 +4026,31 @@
         <v>2</v>
       </c>
       <c r="H34">
-        <v>1.3617313780256672</v>
+        <v>0.89422127560513354</v>
       </c>
       <c r="I34">
-        <v>1.3617313780256672</v>
+        <v>0.89422127560513354</v>
       </c>
       <c r="J34">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="K34">
-        <v>1.25</v>
+        <v>0.8</v>
       </c>
       <c r="L34">
-        <v>1.3780147366022257</v>
+        <v>0.80560294732044513</v>
       </c>
       <c r="M34">
-        <v>1.3780147366022257</v>
+        <v>0.80560294732044513</v>
       </c>
       <c r="N34">
         <v>0</v>
       </c>
       <c r="O34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q34">
         <f t="shared" si="0"/>
@@ -3984,11 +4058,11 @@
       </c>
       <c r="R34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="S34">
         <f t="shared" si="2"/>
-        <v>1.3780147366022257</v>
+        <v>0</v>
       </c>
       <c r="T34">
         <f t="shared" si="3"/>
@@ -3996,18 +4070,18 @@
       </c>
       <c r="U34">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="V34">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="Y34" s="6" t="s">
         <v>112</v>
       </c>
       <c r="Z34" s="7">
         <f>'Optimisation Model'!N20+'Optimisation Model'!O20+'Optimisation Model'!P20</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA34" s="7">
         <v>1</v>
@@ -4039,22 +4113,22 @@
         <v>2</v>
       </c>
       <c r="H35">
-        <v>9.9700036472965464E-2</v>
+        <v>0.24806500729459308</v>
       </c>
       <c r="I35">
-        <v>2.8913010577159985</v>
+        <v>7.1938852115431997</v>
       </c>
       <c r="J35">
-        <v>0.49389719660221698</v>
+        <v>0.51574069682270518</v>
       </c>
       <c r="K35">
-        <v>14.323018701464292</v>
+        <v>14.95648020785845</v>
       </c>
       <c r="L35">
-        <v>0.71245350775939464</v>
+        <v>0.22249070155187894</v>
       </c>
       <c r="M35">
-        <v>20.661151725022446</v>
+        <v>6.4522303450044891</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -4071,7 +4145,7 @@
       </c>
       <c r="R35">
         <f t="shared" si="1"/>
-        <v>0.49389719660221698</v>
+        <v>0.51574069682270518</v>
       </c>
       <c r="S35">
         <f t="shared" si="2"/>
@@ -4126,22 +4200,22 @@
         <v>2</v>
       </c>
       <c r="H36">
-        <v>0.29403581923154187</v>
+        <v>0.37130716384630835</v>
       </c>
       <c r="I36">
-        <v>0.94744875085719049</v>
+        <v>1.1964341946158825</v>
       </c>
       <c r="J36">
-        <v>0.5064059844817137</v>
+        <v>0.42074421197450407</v>
       </c>
       <c r="K36">
-        <v>1.6317526166632996</v>
+        <v>1.3557313496956243</v>
       </c>
       <c r="L36">
-        <v>0.67582200158284778</v>
+        <v>0.26516440031656957</v>
       </c>
       <c r="M36">
-        <v>2.1776486717669541</v>
+        <v>0.85441862324227968</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -4181,7 +4255,7 @@
       </c>
       <c r="Z36" s="7">
         <f>'Optimisation Model'!N22+'Optimisation Model'!O22+'Optimisation Model'!P22</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA36" s="7">
         <v>1</v>
@@ -4213,22 +4287,22 @@
         <v>4</v>
       </c>
       <c r="H37">
-        <v>0.2153370346449783</v>
+        <v>7.1192406928995658E-2</v>
       </c>
       <c r="I37">
-        <v>1.2489548009408742</v>
+        <v>0.41291596018817478</v>
       </c>
       <c r="J37">
-        <v>0.18125030861125108</v>
+        <v>7.2500123444500464E-2</v>
       </c>
       <c r="K37">
-        <v>1.0512517899452563</v>
+        <v>0.42050071597810268</v>
       </c>
       <c r="L37">
-        <v>0.70881552076242349</v>
+        <v>0.34176310415248468</v>
       </c>
       <c r="M37">
-        <v>4.1111300204220562</v>
+        <v>1.9822260040844111</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -4268,7 +4342,7 @@
       </c>
       <c r="Z37" s="7">
         <f>'Optimisation Model'!N23+'Optimisation Model'!O23+'Optimisation Model'!P23</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA37" s="7">
         <v>1</v>
@@ -4300,28 +4374,28 @@
         <v>2</v>
       </c>
       <c r="H38">
-        <v>0.33195820496699041</v>
+        <v>0.32264164099339809</v>
       </c>
       <c r="I38">
-        <v>1.3752554205775316</v>
+        <v>1.3366582269726492</v>
       </c>
       <c r="J38">
-        <v>0.4087227668892392</v>
+        <v>0.39076183402842302</v>
       </c>
       <c r="K38">
-        <v>1.6932800342554195</v>
+        <v>1.6188704552606095</v>
       </c>
       <c r="L38">
-        <v>0.75591241989624658</v>
+        <v>0.30618248397924935</v>
       </c>
       <c r="M38">
-        <v>3.1316371681415927</v>
+        <v>1.2684702907711758</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -4332,7 +4406,7 @@
       </c>
       <c r="R38">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.39076183402842302</v>
       </c>
       <c r="S38">
         <f t="shared" si="2"/>
@@ -4344,7 +4418,7 @@
       </c>
       <c r="U38">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V38">
         <f t="shared" si="5"/>
@@ -4387,22 +4461,22 @@
         <v>2</v>
       </c>
       <c r="H39">
-        <v>0.3664221982671183</v>
+        <v>0.25765943965342364</v>
       </c>
       <c r="I39">
-        <v>2.1252487499492858</v>
+        <v>1.4944247499898571</v>
       </c>
       <c r="J39">
-        <v>0.39303807759725007</v>
+        <v>0.26024553406920298</v>
       </c>
       <c r="K39">
-        <v>2.2796208500640502</v>
+        <v>1.5094240976013771</v>
       </c>
       <c r="L39">
-        <v>0.70562668675076878</v>
+        <v>0.35112533735015378</v>
       </c>
       <c r="M39">
-        <v>4.0926347831544589</v>
+        <v>2.0365269566308917</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -4442,7 +4516,7 @@
       </c>
       <c r="Z39" s="7">
         <f>'Optimisation Model'!N25+'Optimisation Model'!O25+'Optimisation Model'!P25</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA39" s="7">
         <v>1</v>
@@ -4474,22 +4548,22 @@
         <v>2</v>
       </c>
       <c r="H40">
-        <v>0.30631311569999464</v>
+        <v>0.2237626231399989</v>
       </c>
       <c r="I40">
-        <v>1.2690114793285492</v>
+        <v>0.92701658157999534</v>
       </c>
       <c r="J40">
-        <v>0.48600801775843239</v>
+        <v>0.29743351013367614</v>
       </c>
       <c r="K40">
-        <v>2.0134617878563628</v>
+        <v>1.2322245419823725</v>
       </c>
       <c r="L40">
-        <v>0.71748866824951441</v>
+        <v>0.21849773364990288</v>
       </c>
       <c r="M40">
-        <v>2.9724530541765595</v>
+        <v>0.90520489654959757</v>
       </c>
       <c r="N40">
         <v>0</v>
@@ -4529,7 +4603,7 @@
       </c>
       <c r="Z40" s="7">
         <f>'Optimisation Model'!N26+'Optimisation Model'!O26+'Optimisation Model'!P26</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA40" s="7">
         <v>1</v>
@@ -4561,22 +4635,22 @@
         <v>4</v>
       </c>
       <c r="H41">
-        <v>0.1653959000477046</v>
+        <v>0.18932918000954091</v>
       </c>
       <c r="I41">
-        <v>0.9592962202766866</v>
+        <v>1.0981092440553373</v>
       </c>
       <c r="J41">
-        <v>0.17625293792818419</v>
+        <v>0.15534966001975875</v>
       </c>
       <c r="K41">
-        <v>1.0222670399834684</v>
+        <v>0.9010280281146007</v>
       </c>
       <c r="L41">
-        <v>0.80258248032298851</v>
+        <v>0.39551649606459777</v>
       </c>
       <c r="M41">
-        <v>4.6549783858733331</v>
+        <v>2.2939956771746668</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -4648,22 +4722,22 @@
         <v>5</v>
       </c>
       <c r="H42">
-        <v>0.60504053545136371</v>
+        <v>0.23350810709027275</v>
       </c>
       <c r="I42">
-        <v>2.5065965040127924</v>
+        <v>0.96739072937398707</v>
       </c>
       <c r="J42">
-        <v>0.23680732267137705</v>
+        <v>0.14017747452309637</v>
       </c>
       <c r="K42">
-        <v>0.98105890820999064</v>
+        <v>0.58073525159568495</v>
       </c>
       <c r="L42">
-        <v>0.75657745452808334</v>
+        <v>0.45131549090561668</v>
       </c>
       <c r="M42">
-        <v>3.1343923116163452</v>
+        <v>1.8697356051804119</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -4703,7 +4777,7 @@
       </c>
       <c r="Z42" s="7">
         <f>'Optimisation Model'!N28+'Optimisation Model'!O28+'Optimisation Model'!P28</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA42" s="7">
         <v>1</v>
@@ -4735,22 +4809,22 @@
         <v>5</v>
       </c>
       <c r="H43">
-        <v>0.39092828481737912</v>
+        <v>0.24693565696347577</v>
       </c>
       <c r="I43">
-        <v>2.2673840519407986</v>
+        <v>1.4322268103881595</v>
       </c>
       <c r="J43">
-        <v>0.14290120906817802</v>
+        <v>6.6251392718180424E-2</v>
       </c>
       <c r="K43">
-        <v>0.82882701259543246</v>
+        <v>0.38425807776544646</v>
       </c>
       <c r="L43">
-        <v>0.84759095378564397</v>
+        <v>0.46951819075712875</v>
       </c>
       <c r="M43">
-        <v>4.9160275319567344</v>
+        <v>2.7232055063913467</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -4759,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="P43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q43">
         <f t="shared" si="0"/>
@@ -4771,7 +4845,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.46951819075712875</v>
       </c>
       <c r="T43">
         <f t="shared" si="3"/>
@@ -4783,7 +4857,7 @@
       </c>
       <c r="V43">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y43" s="6" t="s">
         <v>121</v>
@@ -4822,22 +4896,22 @@
         <v>5</v>
       </c>
       <c r="H44">
-        <v>0.44501554391124409</v>
+        <v>0.1733781087822488</v>
       </c>
       <c r="I44">
-        <v>1.4339389748251199</v>
+        <v>0.55866279496502391</v>
       </c>
       <c r="J44">
-        <v>0.23475202401835771</v>
+        <v>0.12117353688007038</v>
       </c>
       <c r="K44">
-        <v>0.75642318850359702</v>
+        <v>0.39044806328022674</v>
       </c>
       <c r="L44">
-        <v>0.89263051382314607</v>
+        <v>0.50352610276462917</v>
       </c>
       <c r="M44">
-        <v>2.8762538778745816</v>
+        <v>1.6224729977971384</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -4909,22 +4983,22 @@
         <v>4</v>
       </c>
       <c r="H45">
-        <v>0.41102393294975165</v>
+        <v>0.31032978658995036</v>
       </c>
       <c r="I45">
-        <v>2.3839388111085595</v>
+        <v>1.7999127622217119</v>
       </c>
       <c r="J45">
-        <v>0.25921776975377847</v>
+        <v>0.31277801699242058</v>
       </c>
       <c r="K45">
-        <v>1.5034630645719149</v>
+        <v>1.8141124985560393</v>
       </c>
       <c r="L45">
-        <v>0.79927133230494429</v>
+        <v>0.31485426646098885</v>
       </c>
       <c r="M45">
-        <v>4.6357737273686768</v>
+        <v>1.8261547454737352</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -4996,22 +5070,22 @@
         <v>2</v>
       </c>
       <c r="H46">
-        <v>0.43326650293321595</v>
+        <v>0.27102830058664318</v>
       </c>
       <c r="I46">
-        <v>2.5129457170126521</v>
+        <v>1.5719641434025304</v>
       </c>
       <c r="J46">
-        <v>0.39855345229320926</v>
+        <v>0.27154259303849593</v>
       </c>
       <c r="K46">
-        <v>2.3116100233006134</v>
+        <v>1.5749470396232763</v>
       </c>
       <c r="L46">
-        <v>0.76775733581741978</v>
+        <v>0.38855146716348399</v>
       </c>
       <c r="M46">
-        <v>4.4529925477410348</v>
+        <v>2.253598509548207</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -5083,22 +5157,22 @@
         <v>2</v>
       </c>
       <c r="H47">
-        <v>0.58594251182027657</v>
+        <v>0.48593850236405534</v>
       </c>
       <c r="I47">
-        <v>0.89433330751515905</v>
+        <v>0.74169560887145292</v>
       </c>
       <c r="J47">
-        <v>0.85727634784659756</v>
+        <v>0.55200144822954833</v>
       </c>
       <c r="K47">
-        <v>1.3084744256605962</v>
+        <v>0.84252852624510011</v>
       </c>
       <c r="L47">
-        <v>1.163960020084102</v>
+        <v>0.63779200401682035</v>
       </c>
       <c r="M47">
-        <v>1.7765705569704715</v>
+        <v>0.97347200613093632</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -5170,22 +5244,22 @@
         <v>2</v>
       </c>
       <c r="H48">
-        <v>0.21912462924523615</v>
+        <v>0.14382492584904724</v>
       </c>
       <c r="I48">
-        <v>6.3546142481118482</v>
+        <v>4.1709228496223698</v>
       </c>
       <c r="J48">
-        <v>0.1512327965964127</v>
+        <v>0.12715978530523192</v>
       </c>
       <c r="K48">
-        <v>4.385751101295968</v>
+        <v>3.6876337738517257</v>
       </c>
       <c r="L48">
-        <v>0.67427133230494429</v>
+        <v>0.29485426646098889</v>
       </c>
       <c r="M48">
-        <v>19.553868636843386</v>
+        <v>8.5507737273686786</v>
       </c>
       <c r="N48">
         <v>0</v>
@@ -5257,22 +5331,22 @@
         <v>2</v>
       </c>
       <c r="H49">
-        <v>0.65173629858518556</v>
+        <v>0.44909725971703718</v>
       </c>
       <c r="I49">
-        <v>1.4538732814592601</v>
+        <v>1.0018323485995444</v>
       </c>
       <c r="J49">
-        <v>0.60537090670791693</v>
+        <v>0.46942108995589438</v>
       </c>
       <c r="K49">
-        <v>1.3504427918868915</v>
+        <v>1.0471701237477644</v>
       </c>
       <c r="L49">
-        <v>0.9500018669952579</v>
+        <v>0.51000037339905158</v>
       </c>
       <c r="M49">
-        <v>2.1192349340663443</v>
+        <v>1.1376931406594226</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -5344,25 +5418,25 @@
         <v>4</v>
       </c>
       <c r="H50">
-        <v>0.69850492586595025</v>
+        <v>0.40845098517319001</v>
       </c>
       <c r="I50">
-        <v>4.0513285700225108</v>
+        <v>2.3690157140045018</v>
       </c>
       <c r="J50">
-        <v>0.27878682826069007</v>
+        <v>0.26302988281942774</v>
       </c>
       <c r="K50">
-        <v>1.6169636039120023</v>
+        <v>1.5255733203526809</v>
       </c>
       <c r="L50">
-        <v>0.77103492956193309</v>
+        <v>0.32420698591238661</v>
       </c>
       <c r="M50">
-        <v>4.4720025914592112</v>
+        <v>1.8804005182918422</v>
       </c>
       <c r="N50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -5372,7 +5446,7 @@
       </c>
       <c r="Q50">
         <f t="shared" si="0"/>
-        <v>0.69850492586595025</v>
+        <v>0</v>
       </c>
       <c r="R50">
         <f t="shared" si="1"/>
@@ -5384,7 +5458,7 @@
       </c>
       <c r="T50">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U50">
         <f t="shared" si="4"/>
@@ -5431,22 +5505,22 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>1.2882177308481522</v>
+        <v>0.79514354616963034</v>
       </c>
       <c r="I51">
-        <v>2.4905542796397606</v>
+        <v>1.5372775225946185</v>
       </c>
       <c r="J51">
-        <v>0.72278685753135119</v>
+        <v>0.55275110664890437</v>
       </c>
       <c r="K51">
-        <v>1.3973879245606122</v>
+        <v>1.068652139521215</v>
       </c>
       <c r="L51">
-        <v>0.98525073746312697</v>
+        <v>0.47705014749262536</v>
       </c>
       <c r="M51">
-        <v>1.9048180924287119</v>
+        <v>0.92229695181907567</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -5459,7 +5533,7 @@
       </c>
       <c r="Q51">
         <f t="shared" si="0"/>
-        <v>1.2882177308481522</v>
+        <v>0.79514354616963034</v>
       </c>
       <c r="R51">
         <f t="shared" si="1"/>
@@ -5518,25 +5592,25 @@
         <v>3</v>
       </c>
       <c r="H52">
-        <v>1.2006214232844359</v>
+        <v>0.56512428465688724</v>
       </c>
       <c r="I52">
-        <v>1.8325274355394021</v>
+        <v>0.86255811868682797</v>
       </c>
       <c r="J52">
-        <v>0.72302888781099484</v>
+        <v>0.40133276724561023</v>
       </c>
       <c r="K52">
-        <v>1.1035704077115185</v>
+        <v>0.612560539480142</v>
       </c>
       <c r="L52">
-        <v>0.78055824099551319</v>
+        <v>0.41611164819910268</v>
       </c>
       <c r="M52">
-        <v>1.191378367835257</v>
+        <v>0.63511777883020937</v>
       </c>
       <c r="N52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -5546,7 +5620,7 @@
       </c>
       <c r="Q52">
         <f t="shared" si="0"/>
-        <v>1.2006214232844359</v>
+        <v>0</v>
       </c>
       <c r="R52">
         <f t="shared" si="1"/>
@@ -5558,7 +5632,7 @@
       </c>
       <c r="T52">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U52">
         <f t="shared" si="4"/>
@@ -5573,7 +5647,7 @@
       </c>
       <c r="Z52" s="7">
         <f>'Optimisation Model'!N38+'Optimisation Model'!O38+'Optimisation Model'!P38</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA52" s="7">
         <v>1</v>
@@ -5605,22 +5679,22 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>0.75562126167382737</v>
+        <v>0.4354992523347655</v>
       </c>
       <c r="I53">
-        <v>1.6856166606569996</v>
+        <v>0.97149833213139991</v>
       </c>
       <c r="J53">
-        <v>0.88842022423216283</v>
+        <v>0.70082263514741117</v>
       </c>
       <c r="K53">
-        <v>1.9818605002102094</v>
+        <v>1.5633735707134557</v>
       </c>
       <c r="L53">
-        <v>1.1010906691507532</v>
+        <v>0.57521813383015075</v>
       </c>
       <c r="M53">
-        <v>2.456279185028603</v>
+        <v>1.2831789139287979</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -5637,7 +5711,7 @@
       </c>
       <c r="R53">
         <f t="shared" si="1"/>
-        <v>0.88842022423216283</v>
+        <v>0.70082263514741117</v>
       </c>
       <c r="S53">
         <f t="shared" si="2"/>
@@ -5692,22 +5766,22 @@
         <v>4</v>
       </c>
       <c r="H54">
-        <v>9.375E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="I54">
-        <v>0.38839285714285715</v>
+        <v>0.31071428571428567</v>
       </c>
       <c r="J54">
-        <v>4.5454545454545456E-2</v>
+        <v>3.6363636363636369E-2</v>
       </c>
       <c r="K54">
-        <v>0.18831168831168832</v>
+        <v>0.15064935064935067</v>
       </c>
       <c r="L54">
-        <v>0.125</v>
+        <v>0.3</v>
       </c>
       <c r="M54">
-        <v>0.51785714285714279</v>
+        <v>1.2428571428571427</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -5779,22 +5853,22 @@
         <v>5</v>
       </c>
       <c r="H55">
-        <v>0.55867709655270115</v>
+        <v>0.19611041931054027</v>
       </c>
       <c r="I55">
-        <v>1.4728759818207577</v>
+        <v>0.51701837818233343</v>
       </c>
       <c r="J55">
-        <v>0.25734530047731052</v>
+        <v>0.13021084746365158</v>
       </c>
       <c r="K55">
-        <v>0.678455792167455</v>
+        <v>0.34328314331326326</v>
       </c>
       <c r="L55">
-        <v>0.75760466563827766</v>
+        <v>0.40152093312765552</v>
       </c>
       <c r="M55">
-        <v>1.9973213912281866</v>
+        <v>1.0585551873365464</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -5866,22 +5940,22 @@
         <v>5</v>
       </c>
       <c r="H56">
-        <v>0.37407761221517716</v>
+        <v>0.13106552244303543</v>
       </c>
       <c r="I56">
-        <v>1.5497501077485911</v>
+        <v>0.54298573583543253</v>
       </c>
       <c r="J56">
-        <v>0.17980668981739983</v>
+        <v>9.0104494108778355E-2</v>
       </c>
       <c r="K56">
-        <v>0.74491342924351356</v>
+        <v>0.37329004702208174</v>
       </c>
       <c r="L56">
-        <v>0.81270159622859972</v>
+        <v>0.43754031924571996</v>
       </c>
       <c r="M56">
-        <v>3.366906612947056</v>
+        <v>1.8126670368751254</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -5953,22 +6027,22 @@
         <v>3</v>
       </c>
       <c r="H57">
-        <v>0.33238593052035581</v>
+        <v>0.22897718610407114</v>
       </c>
       <c r="I57">
-        <v>0.6426127990060212</v>
+        <v>0.44268922646787084</v>
       </c>
       <c r="J57">
-        <v>0.56962004580964121</v>
+        <v>0.33996923044506855</v>
       </c>
       <c r="K57">
-        <v>1.1012654218986395</v>
+        <v>0.65727384552713253</v>
       </c>
       <c r="L57">
-        <v>0.67202297779847853</v>
+        <v>0.23440459555969573</v>
       </c>
       <c r="M57">
-        <v>1.2992444237437251</v>
+        <v>0.45318221808207837</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -6008,7 +6082,7 @@
       </c>
       <c r="Z57" s="7">
         <f>'Optimisation Model'!N43+'Optimisation Model'!O43+'Optimisation Model'!P43</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA57" s="7">
         <v>1</v>
@@ -6040,22 +6114,22 @@
         <v>4</v>
       </c>
       <c r="H58">
-        <v>1.234375</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="I58">
-        <v>3.2542613636363638</v>
+        <v>1.5488636363636366</v>
       </c>
       <c r="J58">
-        <v>0.48530064631722791</v>
+        <v>0.43957480398143667</v>
       </c>
       <c r="K58">
-        <v>1.2794289766545099</v>
+        <v>1.158879028678333</v>
       </c>
       <c r="L58">
-        <v>0.9552123470381505</v>
+        <v>0.42104246940763007</v>
       </c>
       <c r="M58">
-        <v>2.5182870967369424</v>
+        <v>1.1100210557110248</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -6068,7 +6142,7 @@
       </c>
       <c r="Q58">
         <f t="shared" si="0"/>
-        <v>1.234375</v>
+        <v>0.58750000000000002</v>
       </c>
       <c r="R58">
         <f t="shared" si="1"/>
@@ -6127,22 +6201,22 @@
         <v>2</v>
       </c>
       <c r="H59">
-        <v>0.44291602225908799</v>
+        <v>0.3729582044518176</v>
       </c>
       <c r="I59">
-        <v>1.1676876950466866</v>
+        <v>0.9832534481002464</v>
       </c>
       <c r="J59">
-        <v>0.32388584957503391</v>
+        <v>0.35682706710274092</v>
       </c>
       <c r="K59">
-        <v>0.85388087615236219</v>
+        <v>0.94072590417995339</v>
       </c>
       <c r="L59">
-        <v>0.60034961214902227</v>
+        <v>0.20006992242980448</v>
       </c>
       <c r="M59">
-        <v>1.5827398865746951</v>
+        <v>0.52745706822403005</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -6214,22 +6288,22 @@
         <v>2</v>
       </c>
       <c r="H60">
-        <v>0.69181830405584832</v>
+        <v>0.40711366081116962</v>
       </c>
       <c r="I60">
-        <v>1.3375153878413066</v>
+        <v>0.78708641090159459</v>
       </c>
       <c r="J60">
-        <v>0.67206115420114387</v>
+        <v>0.35367294652894243</v>
       </c>
       <c r="K60">
-        <v>1.2993182314555447</v>
+        <v>0.68376769662262205</v>
       </c>
       <c r="L60">
-        <v>0.75883519135731525</v>
+        <v>0.38676703827146308</v>
       </c>
       <c r="M60">
-        <v>1.4670813699574761</v>
+        <v>0.74774960732482854</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -6301,25 +6375,25 @@
         <v>2</v>
       </c>
       <c r="H61">
-        <v>0.70594287255943744</v>
+        <v>0.22556357451188747</v>
       </c>
       <c r="I61">
-        <v>4.0944686608447372</v>
+        <v>1.3082687321689472</v>
       </c>
       <c r="J61">
-        <v>0.22455358895446736</v>
+        <v>9.8912344672696106E-2</v>
       </c>
       <c r="K61">
-        <v>1.3024108159359107</v>
+        <v>0.57369159910163736</v>
       </c>
       <c r="L61">
-        <v>0.77103492956193309</v>
+        <v>0.40420698591238663</v>
       </c>
       <c r="M61">
-        <v>4.4720025914592112</v>
+        <v>2.3444005182918422</v>
       </c>
       <c r="N61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O61">
         <v>0</v>
@@ -6329,7 +6403,7 @@
       </c>
       <c r="Q61">
         <f t="shared" si="0"/>
-        <v>0.70594287255943744</v>
+        <v>0</v>
       </c>
       <c r="R61">
         <f t="shared" si="1"/>
@@ -6341,7 +6415,7 @@
       </c>
       <c r="T61">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="U61">
         <f t="shared" si="4"/>
@@ -6401,7 +6475,7 @@
       </c>
       <c r="Z64" s="7">
         <f>'Optimisation Model'!N50+'Optimisation Model'!O50+'Optimisation Model'!P50</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA64" s="7">
         <v>1</v>
@@ -6431,7 +6505,7 @@
       </c>
       <c r="Z66" s="7">
         <f>'Optimisation Model'!N52+'Optimisation Model'!O52+'Optimisation Model'!P52</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA66" s="7">
         <v>1</v>
@@ -6566,7 +6640,7 @@
       </c>
       <c r="Z75" s="7">
         <f>'Optimisation Model'!N61+'Optimisation Model'!O61+'Optimisation Model'!P61</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA75" s="7">
         <v>1</v>
@@ -6577,9 +6651,19 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="Z8:AB8"/>
+    <mergeCell ref="Z5:AB5"/>
   </mergeCells>
   <conditionalFormatting sqref="N1:P1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:F61">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -6590,33 +6674,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="17.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>155</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated to remove party size from the metric, and include a bonus if the leader picked them
</commit_message>
<xml_diff>
--- a/AinBOptimisationdataModel_LF.xlsx
+++ b/AinBOptimisationdataModel_LF.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="22680" windowHeight="13460"/>
+    <workbookView xWindow="0" yWindow="540" windowWidth="25600" windowHeight="13460"/>
   </bookViews>
   <sheets>
     <sheet name="Optimisation Model" sheetId="1" r:id="rId1"/>
@@ -1174,10 +1174,10 @@
   <dimension ref="A1:AB75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z9" sqref="Z9"/>
+      <selection pane="bottomRight" activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1289,22 +1289,22 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <v>0.2847986837409866</v>
+        <v>0.22609901280573991</v>
       </c>
       <c r="I2">
-        <v>1.6518323656977223</v>
+        <v>1.3113742742732915</v>
       </c>
       <c r="J2">
-        <v>0.44086387350270534</v>
+        <v>0.36075588931486707</v>
       </c>
       <c r="K2">
-        <v>2.557010466315691</v>
+        <v>2.092384158026229</v>
       </c>
       <c r="L2">
-        <v>0.39257460382794812</v>
+        <v>0.41776428620429445</v>
       </c>
       <c r="M2">
-        <v>2.2769327022020991</v>
+        <v>2.4230328599849078</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="R2">
         <f>O2*J2</f>
-        <v>0.44086387350270534</v>
+        <v>0.36075588931486707</v>
       </c>
       <c r="S2">
         <f>L2*P2</f>
@@ -1363,22 +1363,22 @@
         <v>4</v>
       </c>
       <c r="H3">
-        <v>0.2811356412437831</v>
+        <v>0.29835173093283729</v>
       </c>
       <c r="I3">
-        <v>0.62714873815920846</v>
+        <v>0.6655538613117139</v>
       </c>
       <c r="J3">
-        <v>0.39444127085397485</v>
+        <v>0.37846944533056126</v>
       </c>
       <c r="K3">
-        <v>0.87990745036655926</v>
+        <v>0.84427799342971355</v>
       </c>
       <c r="L3">
-        <v>0.59225468915233481</v>
+        <v>0.40974657241980672</v>
       </c>
       <c r="M3">
-        <v>1.3211835373398237</v>
+        <v>0.91405004616726115</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="Z3">
         <f>SUM('Optimisation Model'!Q2:Q61)+SUM('Optimisation Model'!R2:R61)+SUM('Optimisation Model'!S2:S61)</f>
-        <v>9.1738012645278388</v>
+        <v>8.6718981324924087</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -1444,22 +1444,22 @@
         <v>2</v>
       </c>
       <c r="H4">
-        <v>0.31089914216744274</v>
+        <v>0.23942435662558204</v>
       </c>
       <c r="I4">
-        <v>1.8032150245711678</v>
+        <v>1.3886612684283757</v>
       </c>
       <c r="J4">
-        <v>0.3498570680767098</v>
+        <v>0.28112493456712107</v>
       </c>
       <c r="K4">
-        <v>2.0291709948449168</v>
+        <v>1.630524620489302</v>
       </c>
       <c r="L4">
-        <v>0.21685943609796257</v>
+        <v>0.1026445770734719</v>
       </c>
       <c r="M4">
-        <v>1.2577847293681828</v>
+        <v>0.59533854702613698</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1518,22 +1518,22 @@
         <v>4</v>
       </c>
       <c r="H5">
-        <v>3.184965608844418E-2</v>
+        <v>2.3887242066333133E-2</v>
       </c>
       <c r="I5">
-        <v>0.30788000885496042</v>
+        <v>0.2309100066412203</v>
       </c>
       <c r="J5">
-        <v>0.12741648165722569</v>
+        <v>0.11148942145007246</v>
       </c>
       <c r="K5">
-        <v>1.2316926560198482</v>
+        <v>1.0777310740173671</v>
       </c>
       <c r="L5">
-        <v>0.37655869633702777</v>
+        <v>0.28797457780832636</v>
       </c>
       <c r="M5">
-        <v>3.6400673979246019</v>
+        <v>2.7837542521471548</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1597,22 +1597,22 @@
         <v>4</v>
       </c>
       <c r="H6">
-        <v>9.2836670700066307E-2</v>
+        <v>7.5877503025049725E-2</v>
       </c>
       <c r="I6">
-        <v>0.29914038336688031</v>
+        <v>0.24449417641404911</v>
       </c>
       <c r="J6">
-        <v>0.15167002600181859</v>
+        <v>0.13271127275159122</v>
       </c>
       <c r="K6">
-        <v>0.48871452822808209</v>
+        <v>0.42762521219957172</v>
       </c>
       <c r="L6">
-        <v>0.42618248397924935</v>
+        <v>0.33630352965110366</v>
       </c>
       <c r="M6">
-        <v>1.3732546705998034</v>
+        <v>1.0836447066535562</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -1680,22 +1680,22 @@
         <v>2</v>
       </c>
       <c r="H7">
-        <v>0.30712329075580341</v>
+        <v>0.26784246806685258</v>
       </c>
       <c r="I7">
-        <v>0.80968867562893632</v>
+        <v>0.70613014308533861</v>
       </c>
       <c r="J7">
-        <v>0.30109514033778301</v>
+        <v>0.2634582477955601</v>
       </c>
       <c r="K7">
-        <v>0.79379627907233707</v>
+        <v>0.69457174418829482</v>
       </c>
       <c r="L7">
-        <v>0.62618248397924936</v>
+        <v>0.51963686298443701</v>
       </c>
       <c r="M7">
-        <v>1.6508447304907483</v>
+        <v>1.3699517296862431</v>
       </c>
       <c r="N7">
         <v>0</v>
@@ -1767,22 +1767,22 @@
         <v>2</v>
       </c>
       <c r="H8">
-        <v>0.69853556200993083</v>
+        <v>0.73640167150744817</v>
       </c>
       <c r="I8">
-        <v>1.3505020865525328</v>
+        <v>1.423709898247733</v>
       </c>
       <c r="J8">
-        <v>0.62374130788749327</v>
+        <v>0.6374403110682233</v>
       </c>
       <c r="K8">
-        <v>1.2058998619158203</v>
+        <v>1.2323846013985649</v>
       </c>
       <c r="L8">
-        <v>0.55836169729975038</v>
+        <v>0.49099349519703506</v>
       </c>
       <c r="M8">
-        <v>1.0794992814461839</v>
+        <v>0.9492540907142677</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>0.69853556200993083</v>
+        <v>0.73640167150744817</v>
       </c>
       <c r="R8">
         <f t="shared" si="1"/>
@@ -1854,22 +1854,22 @@
         <v>2</v>
       </c>
       <c r="H9">
-        <v>0.13929388335927451</v>
+        <v>0.11697041251945589</v>
       </c>
       <c r="I9">
-        <v>4.0395226174189611</v>
+        <v>3.3921419630642209</v>
       </c>
       <c r="J9">
-        <v>0.15305985349971105</v>
+        <v>0.13392737181224712</v>
       </c>
       <c r="K9">
-        <v>4.4387357514916204</v>
+        <v>3.8838937825551665</v>
       </c>
       <c r="L9">
-        <v>0.46884982939793102</v>
+        <v>0.3738595942706705</v>
       </c>
       <c r="M9">
-        <v>13.59664505254</v>
+        <v>10.841928233849444</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1890,7 +1890,7 @@
       </c>
       <c r="S9">
         <f t="shared" si="2"/>
-        <v>0.46884982939793102</v>
+        <v>0.3738595942706705</v>
       </c>
       <c r="T9">
         <f t="shared" si="3"/>
@@ -1941,22 +1941,22 @@
         <v>4</v>
       </c>
       <c r="H10">
-        <v>0.20600108506777848</v>
+        <v>0.16700081380083387</v>
       </c>
       <c r="I10">
-        <v>0.66378127410728616</v>
+        <v>0.53811373335824242</v>
       </c>
       <c r="J10">
-        <v>0.16238537489058091</v>
+        <v>0.14208720302925831</v>
       </c>
       <c r="K10">
-        <v>0.52324176353631624</v>
+        <v>0.45783654309427679</v>
       </c>
       <c r="L10">
-        <v>0.46249009135446312</v>
+        <v>0.36908979073806958</v>
       </c>
       <c r="M10">
-        <v>1.4902458499199367</v>
+        <v>1.1892893257115575</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -2028,22 +2028,22 @@
         <v>2</v>
       </c>
       <c r="H11">
-        <v>0.11495733615225766</v>
+        <v>9.8718002114193237E-2</v>
       </c>
       <c r="I11">
-        <v>0.47625182120221027</v>
+        <v>0.40897458018737198</v>
       </c>
       <c r="J11">
-        <v>0.20823891471604311</v>
+        <v>0.18220905037653773</v>
       </c>
       <c r="K11">
-        <v>0.86270407525217851</v>
+        <v>0.7548660658456563</v>
       </c>
       <c r="L11">
-        <v>0.42277831486576933</v>
+        <v>0.33375040281599366</v>
       </c>
       <c r="M11">
-        <v>1.7515101615867585</v>
+        <v>1.3826802402376879</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2115,28 +2115,28 @@
         <v>4</v>
       </c>
       <c r="H12">
-        <v>0.27558067065093883</v>
+        <v>0.2129355029882041</v>
       </c>
       <c r="I12">
-        <v>1.1416913498396037</v>
+        <v>0.88216136952255986</v>
       </c>
       <c r="J12">
-        <v>0.34120145147983494</v>
+        <v>0.4235512700448556</v>
       </c>
       <c r="K12">
-        <v>1.4135488704164589</v>
+        <v>1.7547124044715445</v>
       </c>
       <c r="L12">
-        <v>0.37582342468779645</v>
+        <v>0.24964534629362517</v>
       </c>
       <c r="M12">
-        <v>1.5569827594208709</v>
+        <v>1.0342450060735899</v>
       </c>
       <c r="N12">
         <v>0</v>
       </c>
       <c r="O12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P12">
         <v>0</v>
@@ -2147,7 +2147,7 @@
       </c>
       <c r="R12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.4235512700448556</v>
       </c>
       <c r="S12">
         <f t="shared" si="2"/>
@@ -2159,7 +2159,7 @@
       </c>
       <c r="U12">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="V12">
         <f t="shared" si="5"/>
@@ -2202,22 +2202,22 @@
         <v>3</v>
       </c>
       <c r="H13">
-        <v>0.26865463095646591</v>
+        <v>0.20774097321734944</v>
       </c>
       <c r="I13">
-        <v>0.59930648444134704</v>
+        <v>0.46342217102331795</v>
       </c>
       <c r="J13">
-        <v>0.374314668695098</v>
+        <v>0.30252533510821067</v>
       </c>
       <c r="K13">
-        <v>0.8350096455506032</v>
+        <v>0.67486420908754685</v>
       </c>
       <c r="L13">
-        <v>0.28892274935125423</v>
+        <v>0.17335872868010735</v>
       </c>
       <c r="M13">
-        <v>0.64451997932202865</v>
+        <v>0.38672331782485486</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -2289,22 +2289,22 @@
         <v>5</v>
       </c>
       <c r="H14">
-        <v>0.41251520812635073</v>
+        <v>0.29688640609476302</v>
       </c>
       <c r="I14">
-        <v>1.0875400941512883</v>
+        <v>0.78270052515892075</v>
       </c>
       <c r="J14">
-        <v>0.35603426872118205</v>
+        <v>0.28652998513103434</v>
       </c>
       <c r="K14">
-        <v>0.93863579935584363</v>
+        <v>0.75539723352727239</v>
       </c>
       <c r="L14">
-        <v>0.39225468915233486</v>
+        <v>0.30141323908647338</v>
       </c>
       <c r="M14">
-        <v>1.0341259986743374</v>
+        <v>0.79463490304615714</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -2376,22 +2376,22 @@
         <v>3</v>
       </c>
       <c r="H15">
-        <v>0.32499999999999996</v>
+        <v>0.20625000000000002</v>
       </c>
       <c r="I15">
-        <v>0.4960526315789473</v>
+        <v>0.31480263157894739</v>
       </c>
       <c r="J15">
-        <v>0.33330154827453273</v>
+        <v>0.23330552140688274</v>
       </c>
       <c r="K15">
-        <v>0.50872341578744473</v>
+        <v>0.35609790109471579</v>
       </c>
       <c r="L15">
-        <v>0.4933333333333334</v>
+        <v>0.4555555555555556</v>
       </c>
       <c r="M15">
-        <v>0.75298245614035098</v>
+        <v>0.69532163742690067</v>
       </c>
       <c r="N15">
         <v>0</v>
@@ -2463,22 +2463,22 @@
         <v>2</v>
       </c>
       <c r="H16">
-        <v>0.2</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="I16">
-        <v>1.9333333333333336</v>
+        <v>2.7791666666666663</v>
       </c>
       <c r="J16">
-        <v>0.15777271834474105</v>
+        <v>0.22971779521831504</v>
       </c>
       <c r="K16">
-        <v>1.5251362773324968</v>
+        <v>2.2206053537770454</v>
       </c>
       <c r="L16">
-        <v>0.27603383981744312</v>
+        <v>0.2348031576408601</v>
       </c>
       <c r="M16">
-        <v>2.6683271182352835</v>
+        <v>2.269763857194981</v>
       </c>
       <c r="N16">
         <v>0</v>
@@ -2550,22 +2550,22 @@
         <v>5</v>
       </c>
       <c r="H17">
-        <v>0.26760148867129757</v>
+        <v>0.29445111650347322</v>
       </c>
       <c r="I17">
-        <v>0.86227146349640327</v>
+        <v>0.94878693095563593</v>
       </c>
       <c r="J17">
-        <v>0.2966007625154396</v>
+        <v>0.29285900053434299</v>
       </c>
       <c r="K17">
-        <v>0.95571356810530539</v>
+        <v>0.94365677949954963</v>
       </c>
       <c r="L17">
-        <v>0.42021453472780906</v>
+        <v>0.25293867882363458</v>
       </c>
       <c r="M17">
-        <v>1.354024611900718</v>
+        <v>0.81502463176504469</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -2637,22 +2637,22 @@
         <v>2</v>
       </c>
       <c r="H18">
-        <v>0.34732585453294856</v>
+        <v>0.27299439089971145</v>
       </c>
       <c r="I18">
-        <v>0.43793259919371774</v>
+        <v>0.34421031896050575</v>
       </c>
       <c r="J18">
-        <v>0.63410817302586864</v>
+        <v>0.52984465139763504</v>
       </c>
       <c r="K18">
-        <v>0.7995276964239213</v>
+        <v>0.66806499524049634</v>
       </c>
       <c r="L18">
-        <v>0.43340325576313776</v>
+        <v>0.30394133071124224</v>
       </c>
       <c r="M18">
-        <v>0.54646497465786936</v>
+        <v>0.38323037350547934</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -2724,22 +2724,22 @@
         <v>5</v>
       </c>
       <c r="H19">
-        <v>0.21117538552833989</v>
+        <v>0.17713153914625493</v>
       </c>
       <c r="I19">
-        <v>0.55673510730198705</v>
+        <v>0.46698314865830848</v>
       </c>
       <c r="J19">
-        <v>0.19232629380821376</v>
+        <v>0.16828550708218701</v>
       </c>
       <c r="K19">
-        <v>0.50704204731256353</v>
+        <v>0.44366179139849304</v>
       </c>
       <c r="L19">
-        <v>0.57582403488521228</v>
+        <v>0.47075691505279815</v>
       </c>
       <c r="M19">
-        <v>1.5180815465155597</v>
+        <v>1.2410864124119225</v>
       </c>
       <c r="N19">
         <v>0</v>
@@ -2811,22 +2811,22 @@
         <v>2</v>
       </c>
       <c r="H20">
-        <v>0.63286396717541438</v>
+        <v>0.47464797538156084</v>
       </c>
       <c r="I20">
-        <v>0.96595026568879039</v>
+        <v>0.7244626992665929</v>
       </c>
       <c r="J20">
-        <v>0.55255864201470462</v>
+        <v>0.57515547842953318</v>
       </c>
       <c r="K20">
-        <v>0.8433789799171808</v>
+        <v>0.87786888812928754</v>
       </c>
       <c r="L20">
-        <v>0.71080407269959078</v>
+        <v>0.63532527674691541</v>
       </c>
       <c r="M20">
-        <v>1.0849114793835859</v>
+        <v>0.9697070013505551</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -2847,7 +2847,7 @@
       </c>
       <c r="S20">
         <f t="shared" si="2"/>
-        <v>0.71080407269959078</v>
+        <v>0.63532527674691541</v>
       </c>
       <c r="T20">
         <f t="shared" si="3"/>
@@ -2898,22 +2898,22 @@
         <v>2</v>
       </c>
       <c r="H21">
-        <v>0.71319704880310253</v>
+        <v>0.7536477866023269</v>
       </c>
       <c r="I21">
-        <v>1.5909780319453826</v>
+        <v>1.6812142931898062</v>
       </c>
       <c r="J21">
-        <v>0.63568737583234891</v>
+        <v>0.53122645385330536</v>
       </c>
       <c r="K21">
-        <v>1.4180718383952398</v>
+        <v>1.1850436278266043</v>
       </c>
       <c r="L21">
-        <v>0.57767172355667928</v>
+        <v>0.43436490377862064</v>
       </c>
       <c r="M21">
-        <v>1.2886523063956692</v>
+        <v>0.96896786227538445</v>
       </c>
       <c r="N21">
         <v>1</v>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="Q21">
         <f t="shared" si="0"/>
-        <v>0.71319704880310253</v>
+        <v>0.7536477866023269</v>
       </c>
       <c r="R21">
         <f t="shared" si="1"/>
@@ -2985,22 +2985,22 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>0.66129187890187402</v>
+        <v>0.69596890917640553</v>
       </c>
       <c r="I22">
-        <v>1.0093402362186499</v>
+        <v>1.0622683350587243</v>
       </c>
       <c r="J22">
-        <v>0.77647431829920421</v>
+        <v>0.77108169517847025</v>
       </c>
       <c r="K22">
-        <v>1.1851450121408906</v>
+        <v>1.1769141663250335</v>
       </c>
       <c r="L22">
-        <v>0.62277831486576929</v>
+        <v>0.55041706948266034</v>
       </c>
       <c r="M22">
-        <v>0.95055637532143733</v>
+        <v>0.84011026394721844</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -3072,22 +3072,22 @@
         <v>2</v>
       </c>
       <c r="H23">
-        <v>0.35049582747642516</v>
+        <v>0.3316218706073189</v>
       </c>
       <c r="I23">
-        <v>0.67762526645442189</v>
+        <v>0.64113561650748319</v>
       </c>
       <c r="J23">
-        <v>0.57301487351267288</v>
+        <v>0.53472134765692214</v>
       </c>
       <c r="K23">
-        <v>1.1078287554578341</v>
+        <v>1.0337946054700493</v>
       </c>
       <c r="L23">
-        <v>0.64889423729650342</v>
+        <v>0.65278178908348872</v>
       </c>
       <c r="M23">
-        <v>1.2545288587732399</v>
+        <v>1.2620447922280782</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -3108,7 +3108,7 @@
       </c>
       <c r="S23">
         <f t="shared" si="2"/>
-        <v>0.64889423729650342</v>
+        <v>0.65278178908348872</v>
       </c>
       <c r="T23">
         <f t="shared" si="3"/>
@@ -3159,22 +3159,22 @@
         <v>4</v>
       </c>
       <c r="H24">
-        <v>0.2586576433724071</v>
+        <v>0.20024323252930532</v>
       </c>
       <c r="I24">
-        <v>1.500214331559961</v>
+        <v>1.1614107486699707</v>
       </c>
       <c r="J24">
-        <v>0.39097286064611486</v>
+        <v>0.31710125306535047</v>
       </c>
       <c r="K24">
-        <v>2.2676425917474661</v>
+        <v>1.8391872677790326</v>
       </c>
       <c r="L24">
-        <v>0.37643407210170471</v>
+        <v>0.25010333185405631</v>
       </c>
       <c r="M24">
-        <v>2.183317618189887</v>
+        <v>1.4505993247535265</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -3246,22 +3246,22 @@
         <v>2</v>
       </c>
       <c r="H25">
-        <v>0.31481915309018982</v>
+        <v>0.34236436481764237</v>
       </c>
       <c r="I25">
-        <v>1.3042507770879292</v>
+        <v>1.4183666542445184</v>
       </c>
       <c r="J25">
-        <v>0.37627880324814178</v>
+        <v>0.36257728617545737</v>
       </c>
       <c r="K25">
-        <v>1.5588693277423016</v>
+        <v>1.5021058998697518</v>
       </c>
       <c r="L25">
-        <v>0.406208230572078</v>
+        <v>0.39243395070683629</v>
       </c>
       <c r="M25">
-        <v>1.6828626695128945</v>
+        <v>1.6257977957854646</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -3333,22 +3333,22 @@
         <v>2</v>
       </c>
       <c r="H26">
-        <v>0.41518486855441528</v>
+        <v>0.28013865141581146</v>
       </c>
       <c r="I26">
-        <v>0.8026907458718695</v>
+        <v>0.5416013927372354</v>
       </c>
       <c r="J26">
-        <v>0.48074407527512208</v>
+        <v>0.36231773253239852</v>
       </c>
       <c r="K26">
-        <v>0.92943854553190264</v>
+        <v>0.70048094956263707</v>
       </c>
       <c r="L26">
-        <v>0.65000037339905159</v>
+        <v>0.57861139116039983</v>
       </c>
       <c r="M26">
-        <v>1.2566673885714996</v>
+        <v>1.1186486895767729</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -3369,7 +3369,7 @@
       </c>
       <c r="S26">
         <f t="shared" si="2"/>
-        <v>0.65000037339905159</v>
+        <v>0.57861139116039983</v>
       </c>
       <c r="T26">
         <f t="shared" si="3"/>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="Z26" s="7">
         <f>'Optimisation Model'!N12+'Optimisation Model'!O12+'Optimisation Model'!P12</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA26" s="7">
         <v>1</v>
@@ -3420,22 +3420,22 @@
         <v>4</v>
       </c>
       <c r="H27">
-        <v>0.42669680056553327</v>
+        <v>0.33877260042414992</v>
       </c>
       <c r="I27">
-        <v>1.3749119129333849</v>
+        <v>1.0916006013667052</v>
       </c>
       <c r="J27">
-        <v>0.38499543083291282</v>
+        <v>0.31187100197879863</v>
       </c>
       <c r="K27">
-        <v>1.2405408326838301</v>
+        <v>1.0049176730427956</v>
       </c>
       <c r="L27">
-        <v>0.42104246940763007</v>
+        <v>0.2891151853890559</v>
       </c>
       <c r="M27">
-        <v>1.3566924014245858</v>
+        <v>0.93159337514251339</v>
       </c>
       <c r="N27">
         <v>0</v>
@@ -3506,23 +3506,23 @@
       <c r="G28">
         <v>4</v>
       </c>
-      <c r="H28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="I28" t="e">
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="K28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="L28" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="M28" t="e">
-        <v>#N/A</v>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -3591,22 +3591,22 @@
         <v>3</v>
       </c>
       <c r="H29">
-        <v>0.38218833699302746</v>
+        <v>0.44289125274477059</v>
       </c>
       <c r="I29">
-        <v>0.85257398252290739</v>
+        <v>0.98798817919987281</v>
       </c>
       <c r="J29">
-        <v>0.3151530682634972</v>
+        <v>0.36742560139722669</v>
       </c>
       <c r="K29">
-        <v>0.70303376766472447</v>
+        <v>0.81964172619381337</v>
       </c>
       <c r="L29">
-        <v>0.17558941601792089</v>
+        <v>0.14280317312455179</v>
       </c>
       <c r="M29">
-        <v>0.39169946650151583</v>
+        <v>0.31856092466246166</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -3678,22 +3678,22 @@
         <v>2</v>
       </c>
       <c r="H30">
-        <v>0.3207356202148734</v>
+        <v>0.30305171516115509</v>
       </c>
       <c r="I30">
-        <v>0.54713723448419582</v>
+        <v>0.51697057292197046</v>
       </c>
       <c r="J30">
-        <v>0.45352680144649449</v>
+        <v>0.43016928459901593</v>
       </c>
       <c r="K30">
-        <v>0.77366336717343187</v>
+        <v>0.73381819137479198</v>
       </c>
       <c r="L30">
-        <v>0.55226961398711183</v>
+        <v>0.56364665493477828</v>
       </c>
       <c r="M30">
-        <v>0.94210698856624964</v>
+        <v>0.96151488194756307</v>
       </c>
       <c r="N30">
         <v>0</v>
@@ -3765,22 +3765,22 @@
         <v>2</v>
       </c>
       <c r="H31">
-        <v>0.58316936449372525</v>
+        <v>0.49987702337029394</v>
       </c>
       <c r="I31">
-        <v>16.911911570318033</v>
+        <v>14.496433677738525</v>
       </c>
       <c r="J31">
-        <v>0.58848896532928707</v>
+        <v>0.63992784466312613</v>
       </c>
       <c r="K31">
-        <v>17.066179994549326</v>
+        <v>18.557907495230658</v>
       </c>
       <c r="L31">
-        <v>0.65225468915233487</v>
+        <v>0.50141323908647339</v>
       </c>
       <c r="M31">
-        <v>18.915385985417711</v>
+        <v>14.540983933507729</v>
       </c>
       <c r="N31">
         <v>1</v>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="Q31">
         <f t="shared" si="0"/>
-        <v>0.58316936449372525</v>
+        <v>0.49987702337029394</v>
       </c>
       <c r="R31">
         <f t="shared" si="1"/>
@@ -3852,22 +3852,22 @@
         <v>2</v>
       </c>
       <c r="H32">
-        <v>0.27119505608302591</v>
+        <v>0.20339629206226942</v>
       </c>
       <c r="I32">
-        <v>1.5729313252815502</v>
+        <v>1.1796984939611626</v>
       </c>
       <c r="J32">
-        <v>0.30040968016854697</v>
+        <v>0.2378584701474786</v>
       </c>
       <c r="K32">
-        <v>1.7423761449775723</v>
+        <v>1.3795791268553759</v>
       </c>
       <c r="L32">
-        <v>0.38285152409046214</v>
+        <v>0.25491642084562438</v>
       </c>
       <c r="M32">
-        <v>2.2205388397246804</v>
+        <v>1.4785152409046214</v>
       </c>
       <c r="N32">
         <v>0</v>
@@ -3939,22 +3939,22 @@
         <v>5</v>
       </c>
       <c r="H33">
-        <v>4.4672809708826984E-2</v>
+        <v>3.3504607281620233E-2</v>
       </c>
       <c r="I33">
-        <v>0.14394572017288695</v>
+        <v>0.10795929012966519</v>
       </c>
       <c r="J33">
-        <v>0.11982579102595142</v>
+        <v>0.10484756714770747</v>
       </c>
       <c r="K33">
-        <v>0.38610532663917679</v>
+        <v>0.33784216080927965</v>
       </c>
       <c r="L33">
-        <v>0.43226500837120313</v>
+        <v>0.34086542294506894</v>
       </c>
       <c r="M33">
-        <v>1.3928539158627655</v>
+        <v>1.0983441406007777</v>
       </c>
       <c r="N33">
         <v>0</v>
@@ -4026,22 +4026,22 @@
         <v>2</v>
       </c>
       <c r="H34">
-        <v>0.89422127560513354</v>
+        <v>0.7644159567038501</v>
       </c>
       <c r="I34">
-        <v>0.89422127560513354</v>
+        <v>0.7644159567038501</v>
       </c>
       <c r="J34">
-        <v>0.8</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="K34">
-        <v>0.8</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="L34">
-        <v>0.80560294732044513</v>
+        <v>0.7942022104903339</v>
       </c>
       <c r="M34">
-        <v>0.80560294732044513</v>
+        <v>0.7942022104903339</v>
       </c>
       <c r="N34">
         <v>0</v>
@@ -4058,7 +4058,7 @@
       </c>
       <c r="R34">
         <f t="shared" si="1"/>
-        <v>0.8</v>
+        <v>0.67499999999999993</v>
       </c>
       <c r="S34">
         <f t="shared" si="2"/>
@@ -4113,22 +4113,22 @@
         <v>2</v>
       </c>
       <c r="H35">
-        <v>0.24806500729459308</v>
+        <v>0.19229875547094483</v>
       </c>
       <c r="I35">
-        <v>7.1938852115431997</v>
+        <v>5.5766639086573999</v>
       </c>
       <c r="J35">
-        <v>0.51574069682270518</v>
+        <v>0.576273109719867</v>
       </c>
       <c r="K35">
-        <v>14.95648020785845</v>
+        <v>16.711920181876142</v>
       </c>
       <c r="L35">
-        <v>0.22249070155187894</v>
+        <v>0.1068680261639092</v>
       </c>
       <c r="M35">
-        <v>6.4522303450044891</v>
+        <v>3.0991727587533666</v>
       </c>
       <c r="N35">
         <v>0</v>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="R35">
         <f t="shared" si="1"/>
-        <v>0.51574069682270518</v>
+        <v>0.576273109719867</v>
       </c>
       <c r="S35">
         <f t="shared" si="2"/>
@@ -4200,22 +4200,22 @@
         <v>2</v>
       </c>
       <c r="H36">
-        <v>0.37130716384630835</v>
+        <v>0.30348037288473129</v>
       </c>
       <c r="I36">
-        <v>1.1964341946158825</v>
+        <v>0.97788120151746749</v>
       </c>
       <c r="J36">
-        <v>0.42074421197450407</v>
+        <v>0.34315118547769097</v>
       </c>
       <c r="K36">
-        <v>1.3557313496956243</v>
+        <v>1.1057093754281153</v>
       </c>
       <c r="L36">
-        <v>0.26516440031656957</v>
+        <v>0.14998441134853829</v>
       </c>
       <c r="M36">
-        <v>0.85441862324227968</v>
+        <v>0.48328310323417895</v>
       </c>
       <c r="N36">
         <v>0</v>
@@ -4287,22 +4287,22 @@
         <v>4</v>
       </c>
       <c r="H37">
-        <v>7.1192406928995658E-2</v>
+        <v>5.9644305196746746E-2</v>
       </c>
       <c r="I37">
-        <v>0.41291596018817478</v>
+        <v>0.34593697014113112</v>
       </c>
       <c r="J37">
-        <v>7.2500123444500464E-2</v>
+        <v>6.3437608013937899E-2</v>
       </c>
       <c r="K37">
-        <v>0.42050071597810268</v>
+        <v>0.36793812648083979</v>
       </c>
       <c r="L37">
-        <v>0.34176310415248468</v>
+        <v>0.25632232811436351</v>
       </c>
       <c r="M37">
-        <v>1.9822260040844111</v>
+        <v>1.4866695030633081</v>
       </c>
       <c r="N37">
         <v>0</v>
@@ -4374,28 +4374,28 @@
         <v>2</v>
       </c>
       <c r="H38">
-        <v>0.32264164099339809</v>
+        <v>0.25448123074504858</v>
       </c>
       <c r="I38">
-        <v>1.3366582269726492</v>
+        <v>1.0542793845152012</v>
       </c>
       <c r="J38">
-        <v>0.39076183402842302</v>
+        <v>0.31691660477487016</v>
       </c>
       <c r="K38">
-        <v>1.6188704552606095</v>
+        <v>1.3129402197816049</v>
       </c>
       <c r="L38">
-        <v>0.30618248397924935</v>
+        <v>0.18630352965110364</v>
       </c>
       <c r="M38">
-        <v>1.2684702907711758</v>
+        <v>0.7718289085545722</v>
       </c>
       <c r="N38">
         <v>0</v>
       </c>
       <c r="O38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -4406,7 +4406,7 @@
       </c>
       <c r="R38">
         <f t="shared" si="1"/>
-        <v>0.39076183402842302</v>
+        <v>0</v>
       </c>
       <c r="S38">
         <f t="shared" si="2"/>
@@ -4418,7 +4418,7 @@
       </c>
       <c r="U38">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="V38">
         <f t="shared" si="5"/>
@@ -4461,22 +4461,22 @@
         <v>2</v>
       </c>
       <c r="H39">
-        <v>0.25765943965342364</v>
+        <v>0.2869945797400677</v>
       </c>
       <c r="I39">
-        <v>1.4944247499898571</v>
+        <v>1.6645685624923925</v>
       </c>
       <c r="J39">
-        <v>0.26024553406920298</v>
+        <v>0.16938150897721924</v>
       </c>
       <c r="K39">
-        <v>1.5094240976013771</v>
+        <v>0.98241275206787149</v>
       </c>
       <c r="L39">
-        <v>0.35112533735015378</v>
+        <v>0.30445511412372639</v>
       </c>
       <c r="M39">
-        <v>2.0365269566308917</v>
+        <v>1.7658396619176129</v>
       </c>
       <c r="N39">
         <v>0</v>
@@ -4548,22 +4548,22 @@
         <v>2</v>
       </c>
       <c r="H40">
-        <v>0.2237626231399989</v>
+        <v>0.45532196735499919</v>
       </c>
       <c r="I40">
-        <v>0.92701658157999534</v>
+        <v>1.8863338647564252</v>
       </c>
       <c r="J40">
-        <v>0.29743351013367614</v>
+        <v>0.35192098803363325</v>
       </c>
       <c r="K40">
-        <v>1.2322245419823725</v>
+        <v>1.4579583789964805</v>
       </c>
       <c r="L40">
-        <v>0.21849773364990288</v>
+        <v>0.18053996690409385</v>
       </c>
       <c r="M40">
-        <v>0.90520489654959757</v>
+        <v>0.74795129145981731</v>
       </c>
       <c r="N40">
         <v>0</v>
@@ -4635,22 +4635,22 @@
         <v>4</v>
       </c>
       <c r="H41">
-        <v>0.18932918000954091</v>
+        <v>7.9496885007155696E-2</v>
       </c>
       <c r="I41">
-        <v>1.0981092440553373</v>
+        <v>0.46108193304150302</v>
       </c>
       <c r="J41">
-        <v>0.15534966001975875</v>
+        <v>7.7597619183955538E-2</v>
       </c>
       <c r="K41">
-        <v>0.9010280281146007</v>
+        <v>0.45006619126694208</v>
       </c>
       <c r="L41">
-        <v>0.39551649606459777</v>
+        <v>0.34330403871511495</v>
       </c>
       <c r="M41">
-        <v>2.2939956771746668</v>
+        <v>1.9911634245476666</v>
       </c>
       <c r="N41">
         <v>0</v>
@@ -4722,22 +4722,22 @@
         <v>5</v>
       </c>
       <c r="H42">
-        <v>0.23350810709027275</v>
+        <v>0.20013108031770457</v>
       </c>
       <c r="I42">
-        <v>0.96739072937398707</v>
+        <v>0.82911447560191887</v>
       </c>
       <c r="J42">
-        <v>0.14017747452309637</v>
+        <v>0.12265529020770931</v>
       </c>
       <c r="K42">
-        <v>0.58073525159568495</v>
+        <v>0.50814334514622428</v>
       </c>
       <c r="L42">
-        <v>0.45131549090561668</v>
+        <v>0.36070884040143469</v>
       </c>
       <c r="M42">
-        <v>1.8697356051804119</v>
+        <v>1.4943651959488009</v>
       </c>
       <c r="N42">
         <v>0</v>
@@ -4809,22 +4809,22 @@
         <v>5</v>
       </c>
       <c r="H43">
-        <v>0.24693565696347577</v>
+        <v>0.2227017427226069</v>
       </c>
       <c r="I43">
-        <v>1.4322268103881595</v>
+        <v>1.2916701077911199</v>
       </c>
       <c r="J43">
-        <v>6.6251392718180424E-2</v>
+        <v>5.7969968628407857E-2</v>
       </c>
       <c r="K43">
-        <v>0.38425807776544646</v>
+        <v>0.33622581804476553</v>
       </c>
       <c r="L43">
-        <v>0.46951819075712875</v>
+        <v>0.37436086529006884</v>
       </c>
       <c r="M43">
-        <v>2.7232055063913467</v>
+        <v>2.1712930186823991</v>
       </c>
       <c r="N43">
         <v>0</v>
@@ -4845,7 +4845,7 @@
       </c>
       <c r="S43">
         <f t="shared" si="2"/>
-        <v>0.46951819075712875</v>
+        <v>0.37436086529006884</v>
       </c>
       <c r="T43">
         <f t="shared" si="3"/>
@@ -4896,22 +4896,22 @@
         <v>5</v>
       </c>
       <c r="H44">
-        <v>0.1733781087822488</v>
+        <v>0.14878358158668661</v>
       </c>
       <c r="I44">
-        <v>0.55866279496502391</v>
+        <v>0.47941376289043464</v>
       </c>
       <c r="J44">
-        <v>0.12117353688007038</v>
+        <v>0.10602684477006157</v>
       </c>
       <c r="K44">
-        <v>0.39044806328022674</v>
+        <v>0.34164205537019837</v>
       </c>
       <c r="L44">
-        <v>0.50352610276462917</v>
+        <v>0.40542235485124967</v>
       </c>
       <c r="M44">
-        <v>1.6224729977971384</v>
+        <v>1.3063609211873599</v>
       </c>
       <c r="N44">
         <v>0</v>
@@ -4983,22 +4983,22 @@
         <v>4</v>
       </c>
       <c r="H45">
-        <v>0.31032978658995036</v>
+        <v>0.23899733994246278</v>
       </c>
       <c r="I45">
-        <v>1.7999127622217119</v>
+        <v>1.3861845716662839</v>
       </c>
       <c r="J45">
-        <v>0.31277801699242058</v>
+        <v>0.24868076486836793</v>
       </c>
       <c r="K45">
-        <v>1.8141124985560393</v>
+        <v>1.442348436236534</v>
       </c>
       <c r="L45">
-        <v>0.31485426646098885</v>
+        <v>0.19280736651240829</v>
       </c>
       <c r="M45">
-        <v>1.8261547454737352</v>
+        <v>1.1182827257719681</v>
       </c>
       <c r="N45">
         <v>0</v>
@@ -5070,22 +5070,22 @@
         <v>2</v>
       </c>
       <c r="H46">
-        <v>0.27102830058664318</v>
+        <v>0.29702122543998238</v>
       </c>
       <c r="I46">
-        <v>1.5719641434025304</v>
+        <v>1.7227231075518976</v>
       </c>
       <c r="J46">
-        <v>0.27154259303849593</v>
+        <v>0.17926643557535057</v>
       </c>
       <c r="K46">
-        <v>1.5749470396232763</v>
+        <v>1.0397453263370333</v>
       </c>
       <c r="L46">
-        <v>0.38855146716348399</v>
+        <v>0.33808026703927962</v>
       </c>
       <c r="M46">
-        <v>2.253598509548207</v>
+        <v>1.9608655488278217</v>
       </c>
       <c r="N46">
         <v>0</v>
@@ -5157,22 +5157,22 @@
         <v>2</v>
       </c>
       <c r="H47">
-        <v>0.48593850236405534</v>
+        <v>0.40195387677304151</v>
       </c>
       <c r="I47">
-        <v>0.74169560887145292</v>
+        <v>0.61350854875885286</v>
       </c>
       <c r="J47">
-        <v>0.55200144822954833</v>
+        <v>0.45800126720085477</v>
       </c>
       <c r="K47">
-        <v>0.84252852624510011</v>
+        <v>0.69905456572762048</v>
       </c>
       <c r="L47">
-        <v>0.63779200401682035</v>
+        <v>0.49056622523483756</v>
       </c>
       <c r="M47">
-        <v>0.97347200613093632</v>
+        <v>0.74875897535843627</v>
       </c>
       <c r="N47">
         <v>0</v>
@@ -5244,22 +5244,22 @@
         <v>2</v>
       </c>
       <c r="H48">
-        <v>0.14382492584904724</v>
+        <v>3.286869438678542E-2</v>
       </c>
       <c r="I48">
-        <v>4.1709228496223698</v>
+        <v>0.9531921372167772</v>
       </c>
       <c r="J48">
-        <v>0.12715978530523192</v>
+        <v>5.2931478808744575E-2</v>
       </c>
       <c r="K48">
-        <v>3.6876337738517257</v>
+        <v>1.5350128854535927</v>
       </c>
       <c r="L48">
-        <v>0.29485426646098889</v>
+        <v>0.25114069984574161</v>
       </c>
       <c r="M48">
-        <v>8.5507737273686786</v>
+        <v>7.2830802955265064</v>
       </c>
       <c r="N48">
         <v>0</v>
@@ -5331,22 +5331,22 @@
         <v>2</v>
       </c>
       <c r="H49">
-        <v>0.44909725971703718</v>
+        <v>0.33682294478777786</v>
       </c>
       <c r="I49">
-        <v>1.0018323485995444</v>
+        <v>0.75137426144965824</v>
       </c>
       <c r="J49">
-        <v>0.46942108995589438</v>
+        <v>0.38574345371140761</v>
       </c>
       <c r="K49">
-        <v>1.0471701237477644</v>
+        <v>0.86050462751006307</v>
       </c>
       <c r="L49">
-        <v>0.51000037339905158</v>
+        <v>0.41194472449373315</v>
       </c>
       <c r="M49">
-        <v>1.1376931406594226</v>
+        <v>0.91895361617832783</v>
       </c>
       <c r="N49">
         <v>0</v>
@@ -5418,22 +5418,22 @@
         <v>4</v>
       </c>
       <c r="H50">
-        <v>0.40845098517319001</v>
+        <v>0.41883823887989258</v>
       </c>
       <c r="I50">
-        <v>2.3690157140045018</v>
+        <v>2.4292617855033769</v>
       </c>
       <c r="J50">
-        <v>0.26302988281942774</v>
+        <v>0.26348448080033254</v>
       </c>
       <c r="K50">
-        <v>1.5255733203526809</v>
+        <v>1.5282099886419287</v>
       </c>
       <c r="L50">
-        <v>0.32420698591238661</v>
+        <v>0.16426635054540106</v>
       </c>
       <c r="M50">
-        <v>1.8804005182918422</v>
+        <v>0.95274483316332614</v>
       </c>
       <c r="N50">
         <v>0</v>
@@ -5505,22 +5505,22 @@
         <v>2</v>
       </c>
       <c r="H51">
-        <v>0.79514354616963034</v>
+        <v>0.82135765962722285</v>
       </c>
       <c r="I51">
-        <v>1.5372775225946185</v>
+        <v>1.5879581419459641</v>
       </c>
       <c r="J51">
-        <v>0.55275110664890437</v>
+        <v>0.60865721831779129</v>
       </c>
       <c r="K51">
-        <v>1.068652139521215</v>
+        <v>1.1767372887477296</v>
       </c>
       <c r="L51">
-        <v>0.47705014749262536</v>
+        <v>0.34223205506391352</v>
       </c>
       <c r="M51">
-        <v>0.92229695181907567</v>
+        <v>0.66164863979023281</v>
       </c>
       <c r="N51">
         <v>1</v>
@@ -5533,7 +5533,7 @@
       </c>
       <c r="Q51">
         <f t="shared" si="0"/>
-        <v>0.79514354616963034</v>
+        <v>0.82135765962722285</v>
       </c>
       <c r="R51">
         <f t="shared" si="1"/>
@@ -5592,22 +5592,22 @@
         <v>3</v>
       </c>
       <c r="H52">
-        <v>0.56512428465688724</v>
+        <v>0.39884321349266538</v>
       </c>
       <c r="I52">
-        <v>0.86255811868682797</v>
+        <v>0.60876069427827872</v>
       </c>
       <c r="J52">
-        <v>0.40133276724561023</v>
+        <v>0.29283283800657567</v>
       </c>
       <c r="K52">
-        <v>0.612560539480142</v>
+        <v>0.44695538432582604</v>
       </c>
       <c r="L52">
-        <v>0.41611164819910268</v>
+        <v>0.36430595837154922</v>
       </c>
       <c r="M52">
-        <v>0.63511777883020937</v>
+        <v>0.55604593646183831</v>
       </c>
       <c r="N52">
         <v>0</v>
@@ -5647,7 +5647,7 @@
       </c>
       <c r="Z52" s="7">
         <f>'Optimisation Model'!N38+'Optimisation Model'!O38+'Optimisation Model'!P38</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA52" s="7">
         <v>1</v>
@@ -5679,22 +5679,22 @@
         <v>2</v>
       </c>
       <c r="H53">
-        <v>0.4354992523347655</v>
+        <v>0.49537443925107416</v>
       </c>
       <c r="I53">
-        <v>0.97149833213139991</v>
+        <v>1.1050660567908577</v>
       </c>
       <c r="J53">
-        <v>0.70082263514741117</v>
+        <v>0.73821980575398471</v>
       </c>
       <c r="K53">
-        <v>1.5633735707134557</v>
+        <v>1.6467980282204273</v>
       </c>
       <c r="L53">
-        <v>0.57521813383015075</v>
+        <v>0.43252471148372412</v>
       </c>
       <c r="M53">
-        <v>1.2831789139287979</v>
+        <v>0.96486281792523076</v>
       </c>
       <c r="N53">
         <v>0</v>
@@ -5711,7 +5711,7 @@
       </c>
       <c r="R53">
         <f t="shared" si="1"/>
-        <v>0.70082263514741117</v>
+        <v>0.73821980575398471</v>
       </c>
       <c r="S53">
         <f t="shared" si="2"/>
@@ -5766,22 +5766,22 @@
         <v>4</v>
       </c>
       <c r="H54">
-        <v>7.4999999999999997E-2</v>
+        <v>6.8750000000000006E-2</v>
       </c>
       <c r="I54">
-        <v>0.31071428571428567</v>
+        <v>0.28482142857142856</v>
       </c>
       <c r="J54">
-        <v>3.6363636363636369E-2</v>
+        <v>3.1818181818181815E-2</v>
       </c>
       <c r="K54">
-        <v>0.15064935064935067</v>
+        <v>0.13181818181818181</v>
       </c>
       <c r="L54">
-        <v>0.3</v>
+        <v>0.24166666666666667</v>
       </c>
       <c r="M54">
-        <v>1.2428571428571427</v>
+        <v>1.0011904761904762</v>
       </c>
       <c r="N54">
         <v>0</v>
@@ -5853,22 +5853,22 @@
         <v>5</v>
       </c>
       <c r="H55">
-        <v>0.19611041931054027</v>
+        <v>0.16583281448290518</v>
       </c>
       <c r="I55">
-        <v>0.51701837818233343</v>
+        <v>0.43719560181856826</v>
       </c>
       <c r="J55">
-        <v>0.13021084746365158</v>
+        <v>0.11393449153069511</v>
       </c>
       <c r="K55">
-        <v>0.34328314331326326</v>
+        <v>0.30037275039910533</v>
       </c>
       <c r="L55">
-        <v>0.40152093312765552</v>
+        <v>0.31225181095685273</v>
       </c>
       <c r="M55">
-        <v>1.0585551873365464</v>
+        <v>0.82320931979533907</v>
       </c>
       <c r="N55">
         <v>0</v>
@@ -5940,22 +5940,22 @@
         <v>5</v>
       </c>
       <c r="H56">
-        <v>0.13106552244303543</v>
+        <v>0.11079914183227657</v>
       </c>
       <c r="I56">
-        <v>0.54298573583543253</v>
+        <v>0.45902501616228863</v>
       </c>
       <c r="J56">
-        <v>9.0104494108778355E-2</v>
+        <v>7.8841432345181039E-2</v>
       </c>
       <c r="K56">
-        <v>0.37329004702208174</v>
+        <v>0.32662879114432142</v>
       </c>
       <c r="L56">
-        <v>0.43754031924571996</v>
+        <v>0.34482190610095664</v>
       </c>
       <c r="M56">
-        <v>1.8126670368751254</v>
+        <v>1.4285478967039631</v>
       </c>
       <c r="N56">
         <v>0</v>
@@ -6027,22 +6027,22 @@
         <v>3</v>
       </c>
       <c r="H57">
-        <v>0.22897718610407114</v>
+        <v>0.30923288957805339</v>
       </c>
       <c r="I57">
-        <v>0.44268922646787084</v>
+        <v>0.59785025318423657</v>
       </c>
       <c r="J57">
-        <v>0.33996923044506855</v>
+        <v>0.38913974330610168</v>
       </c>
       <c r="K57">
-        <v>0.65727384552713253</v>
+        <v>0.75233683705846321</v>
       </c>
       <c r="L57">
-        <v>0.23440459555969573</v>
+        <v>0.19802566889199402</v>
       </c>
       <c r="M57">
-        <v>0.45318221808207837</v>
+        <v>0.38284962652452176</v>
       </c>
       <c r="N57">
         <v>0</v>
@@ -6114,22 +6114,22 @@
         <v>4</v>
       </c>
       <c r="H58">
-        <v>0.58750000000000002</v>
+        <v>0.47187499999999999</v>
       </c>
       <c r="I58">
-        <v>1.5488636363636366</v>
+        <v>1.244034090909091</v>
       </c>
       <c r="J58">
-        <v>0.43957480398143667</v>
+        <v>0.35962795348375709</v>
       </c>
       <c r="K58">
-        <v>1.158879028678333</v>
+        <v>0.94811005918445057</v>
       </c>
       <c r="L58">
-        <v>0.42104246940763007</v>
+        <v>0.2891151853890559</v>
       </c>
       <c r="M58">
-        <v>1.1100210557110248</v>
+        <v>0.76221276148023831</v>
       </c>
       <c r="N58">
         <v>1</v>
@@ -6142,7 +6142,7 @@
       </c>
       <c r="Q58">
         <f t="shared" si="0"/>
-        <v>0.58750000000000002</v>
+        <v>0.47187499999999999</v>
       </c>
       <c r="R58">
         <f t="shared" si="1"/>
@@ -6201,22 +6201,22 @@
         <v>2</v>
       </c>
       <c r="H59">
-        <v>0.3729582044518176</v>
+        <v>0.29846865333886319</v>
       </c>
       <c r="I59">
-        <v>0.9832534481002464</v>
+        <v>0.78687190425700304</v>
       </c>
       <c r="J59">
-        <v>0.35682706710274092</v>
+        <v>0.28722368371489826</v>
       </c>
       <c r="K59">
-        <v>0.94072590417995339</v>
+        <v>0.75722607524836816</v>
       </c>
       <c r="L59">
-        <v>0.20006992242980448</v>
+        <v>9.0052441822353335E-2</v>
       </c>
       <c r="M59">
-        <v>0.52745706822403005</v>
+        <v>0.23741098298620425</v>
       </c>
       <c r="N59">
         <v>0</v>
@@ -6288,22 +6288,22 @@
         <v>2</v>
       </c>
       <c r="H60">
-        <v>0.40711366081116962</v>
+        <v>0.26783524560837724</v>
       </c>
       <c r="I60">
-        <v>0.78708641090159459</v>
+        <v>0.51781480817619596</v>
       </c>
       <c r="J60">
-        <v>0.35367294652894243</v>
+        <v>0.25113049487949124</v>
       </c>
       <c r="K60">
-        <v>0.68376769662262205</v>
+        <v>0.48551895676701634</v>
       </c>
       <c r="L60">
-        <v>0.38676703827146308</v>
+        <v>0.33674194537026392</v>
       </c>
       <c r="M60">
-        <v>0.74774960732482854</v>
+        <v>0.65103442771584352</v>
       </c>
       <c r="N60">
         <v>0</v>
@@ -6375,22 +6375,22 @@
         <v>2</v>
       </c>
       <c r="H61">
-        <v>0.22556357451188747</v>
+        <v>0.18792268088391562</v>
       </c>
       <c r="I61">
-        <v>1.3082687321689472</v>
+        <v>1.0899515491267104</v>
       </c>
       <c r="J61">
-        <v>9.8912344672696106E-2</v>
+        <v>8.6548301588609086E-2</v>
       </c>
       <c r="K61">
-        <v>0.57369159910163736</v>
+        <v>0.50198014921393264</v>
       </c>
       <c r="L61">
-        <v>0.40420698591238663</v>
+        <v>0.31426635054540109</v>
       </c>
       <c r="M61">
-        <v>2.3444005182918422</v>
+        <v>1.8227448331633263</v>
       </c>
       <c r="N61">
         <v>0</v>

</xml_diff>